<commit_message>
New test added and created a data setup optimized version of the tests
</commit_message>
<xml_diff>
--- a/test/atdd scenarios/Seminar Registration - ATDD Scenarios.xlsx
+++ b/test/atdd scenarios/Seminar Registration - ATDD Scenarios.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2a63c87061b9b9b/Presentations/DOK/2024/Nordic/Presentation 1 - Tip ^0 Tricks for efficient and effective test automation data setup/Code Examples/Seminar Management/test/atdd scenarios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{BB4C36B7-EE5C-4F78-9FD6-35C3B4ED61F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D9C709C-DDA2-49A3-8C0F-B8C657D51A91}"/>
+  <xr:revisionPtr revIDLastSave="230" documentId="13_ncr:1_{BB4C36B7-EE5C-4F78-9FD6-35C3B4ED61F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90CB6D44-EB5C-4656-99CF-E41CBBE6A390}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27720" windowHeight="16440" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
   <sheets>
-    <sheet name="ATDD Scenarios" sheetId="1" r:id="rId1"/>
+    <sheet name="ATDD Scenarios - Posting only" sheetId="2" r:id="rId1"/>
+    <sheet name="ATDD Scenarios" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="123">
   <si>
     <t>Feature</t>
   </si>
@@ -285,22 +286,124 @@
     <t>Room resource</t>
   </si>
   <si>
-    <t>Closed seminar registration with  one participant line</t>
-  </si>
-  <si>
     <t>Seminar registration is removed</t>
   </si>
   <si>
     <t>Posted seminar registration exists</t>
   </si>
   <si>
-    <t>Related ledger entries exist</t>
-  </si>
-  <si>
     <t>Press post button on Seminar Registration List</t>
   </si>
   <si>
-    <t>Post seminar registration from Seminar Registration List page</t>
+    <t>Post seminar registration</t>
+  </si>
+  <si>
+    <t>Customer with contact</t>
+  </si>
+  <si>
+    <t>Room related seminar ledger entry exists</t>
+  </si>
+  <si>
+    <t>Instructor related seminar ledger entry exists</t>
+  </si>
+  <si>
+    <t>Customer related seminar ledger entry exists</t>
+  </si>
+  <si>
+    <t>Instructor related resource ledger entry exists</t>
+  </si>
+  <si>
+    <t>Room related resource ledger entry exists</t>
+  </si>
+  <si>
+    <t>Customer with company contact</t>
+  </si>
+  <si>
+    <t>Person contact for customer</t>
+  </si>
+  <si>
+    <t>Post closed seminar registration from Seminar Registration List page</t>
+  </si>
+  <si>
+    <t>Post closed seminar registration</t>
+  </si>
+  <si>
+    <t>Post non-closed seminar registration</t>
+  </si>
+  <si>
+    <t>Status must be equal to closed error thrown</t>
+  </si>
+  <si>
+    <t>Post closed seminar registration with empty posting date</t>
+  </si>
+  <si>
+    <t>Closed seminar registration with one participant line</t>
+  </si>
+  <si>
+    <t>Non-closed seminar registration with one participant line</t>
+  </si>
+  <si>
+    <t>Closed seminar registration with one participant line and empty posting date</t>
+  </si>
+  <si>
+    <t>Posting date must be have value error thrown</t>
+  </si>
+  <si>
+    <t>Post closed seminar registration with empty document date</t>
+  </si>
+  <si>
+    <t>Document date must be have value error thrown</t>
+  </si>
+  <si>
+    <t>Closed seminar registration with one participant line and empty document date</t>
+  </si>
+  <si>
+    <t>Post closed seminar registration with empty seminar number</t>
+  </si>
+  <si>
+    <t>Closed seminar registration with one participant line and empty seminar number</t>
+  </si>
+  <si>
+    <t>Seminar number must be have value error thrown</t>
+  </si>
+  <si>
+    <t>Post closed seminar registration with empty duration</t>
+  </si>
+  <si>
+    <t>Closed seminar registration with one participant line and empty duration</t>
+  </si>
+  <si>
+    <t>Duration must be have value error thrown</t>
+  </si>
+  <si>
+    <t>Post closed seminar registration with empty instructor resource number</t>
+  </si>
+  <si>
+    <t>Closed seminar registration with one participant line and empty instructor resource number</t>
+  </si>
+  <si>
+    <t>Instructor resource number must be have value error thrown</t>
+  </si>
+  <si>
+    <t>Post closed seminar registration with empty room resource number</t>
+  </si>
+  <si>
+    <t>room resource</t>
+  </si>
+  <si>
+    <t>Closed seminar registration with one participant line and empty room resource number</t>
+  </si>
+  <si>
+    <t>Room resource number must be have value error thrown</t>
+  </si>
+  <si>
+    <t>Closed seminar registration with no participant line</t>
+  </si>
+  <si>
+    <t>Post closed seminar registration with noparticipant line</t>
+  </si>
+  <si>
+    <t>Error thrown</t>
   </si>
 </sst>
 </file>
@@ -393,7 +496,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -460,7 +563,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -470,7 +572,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -485,7 +586,7 @@
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="32">
     <dxf>
       <font>
         <b/>
@@ -506,6 +607,33 @@
         <i val="0"/>
         <color rgb="FF0070C0"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -540,26 +668,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -576,11 +684,67 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -659,8 +823,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:L82" totalsRowShown="0" headerRowDxfId="21">
-  <autoFilter ref="A1:L82" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{22F2C4D7-A7F8-46C0-960F-675A8BCE1D8D}" name="Table293" displayName="Table293" ref="A1:L95" totalsRowShown="0" headerRowDxfId="31">
+  <autoFilter ref="A1:L95" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{3C5A203A-70AF-48EA-9EC7-2C4C4E6D6F0C}" name="Feature"/>
+    <tableColumn id="9" xr3:uid="{B34F943B-2E52-4D5D-96D0-D87B15881916}" name="Sub Feature"/>
+    <tableColumn id="10" xr3:uid="{A0208F55-2DF5-4EDF-97BB-87961D00BE5F}" name="UI" dataDxfId="30"/>
+    <tableColumn id="11" xr3:uid="{7EF33F50-B861-4283-B39A-0F5ECD0862B3}" name="Positve-Negative" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{7C738EFA-3322-4B32-8D39-AA9FB9502075}" name="Scenario" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{3C427682-4F91-4A08-B38A-C00770BC106B}" name="Given-When-Then (Tag)"/>
+    <tableColumn id="5" xr3:uid="{01853C33-EDE0-4B36-AA3B-39AAD27652E3}" name="Given-When-Then (Description)" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{6E358100-3DC1-4410-B65B-D3B7C70DEFC8}" name="Scenario #" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{C1DA78B7-7F2D-4AA4-B547-D3498D52C14E}" name="ATDD Format" dataDxfId="25">
+      <calculatedColumnFormula>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{658005E7-A551-4BA0-9828-C11EC987CE85}" name="Code Format" dataDxfId="24">
+      <calculatedColumnFormula>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="12" xr3:uid="{65087EAD-1650-4D9F-9EDC-940759928B5C}" name="ATDD.TestScriptor Format" dataDxfId="23">
+      <calculatedColumnFormula>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{92D3DED7-99D4-43F1-BAD2-573461C8D8F4}" name="Notes" dataDxfId="22"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D26859EB-C8DA-46B9-9E4C-0C2909BE7347}" name="Table29" displayName="Table29" ref="A1:L73" totalsRowShown="0" headerRowDxfId="21">
+  <autoFilter ref="A1:L73" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{94AE38D3-5B70-43B1-956A-6DFBCCC3FA71}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{39B338AE-1DE7-47E0-9DFF-EB558B693D9E}" name="Sub Feature"/>
@@ -981,11 +1172,2924 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7684FF22-50C0-48D3-B42F-054142E19464}">
+  <dimension ref="A1:L96"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" customWidth="1"/>
+    <col min="7" max="7" width="41.5703125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="12" customWidth="1"/>
+    <col min="9" max="10" width="48.42578125" style="11" customWidth="1"/>
+    <col min="11" max="11" width="48.42578125" style="14" customWidth="1"/>
+    <col min="12" max="12" width="47.7109375" style="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="7" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[FEATURE] Seminar Registration Registration</v>
+      </c>
+      <c r="J2" s="9" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[FEATURE] Seminar Registration Registration</v>
+      </c>
+      <c r="K2" s="15" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Feature 'Seminar Registration' {</v>
+      </c>
+      <c r="L2" s="7"/>
+    </row>
+    <row r="3" spans="1:12" s="18" customFormat="1" ht="39.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="19"/>
+      <c r="E3" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" s="20"/>
+      <c r="H3" s="21">
+        <v>70</v>
+      </c>
+      <c r="I3" s="20" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0070] Post closed seminar registration from Seminar Registration List page</v>
+      </c>
+      <c r="J3" s="22" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0070] Post closed seminar registration from Seminar Registration List page</v>
+      </c>
+      <c r="K3" s="23" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0070 'Post closed seminar registration from Seminar Registration List page' {</v>
+      </c>
+      <c r="L3" s="20"/>
+    </row>
+    <row r="4" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="12">
+        <v>70</v>
+      </c>
+      <c r="I4" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Seminar</v>
+      </c>
+      <c r="J4" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Seminar</v>
+      </c>
+      <c r="K4" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Seminar'</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="H5" s="12">
+        <v>70</v>
+      </c>
+      <c r="I5" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Instructor resource</v>
+      </c>
+      <c r="J5" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Instructor resource</v>
+      </c>
+      <c r="K5" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Instructor resource'</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6" s="12">
+        <v>70</v>
+      </c>
+      <c r="I6" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Room resource</v>
+      </c>
+      <c r="J6" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Room resource</v>
+      </c>
+      <c r="K6" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Room resource'</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="H7" s="12">
+        <v>70</v>
+      </c>
+      <c r="I7" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Customer with company contact</v>
+      </c>
+      <c r="J7" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Customer with company contact</v>
+      </c>
+      <c r="K7" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Customer with company contact'</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H8" s="12">
+        <v>70</v>
+      </c>
+      <c r="I8" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Person contact for customer</v>
+      </c>
+      <c r="J8" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Person contact for customer</v>
+      </c>
+      <c r="K8" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Person contact for customer'</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H9" s="12">
+        <v>70</v>
+      </c>
+      <c r="I9" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Closed seminar registration with one participant line</v>
+      </c>
+      <c r="J9" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Closed seminar registration with one participant line</v>
+      </c>
+      <c r="K9" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Closed seminar registration with one participant line'</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="H10" s="12">
+        <v>70</v>
+      </c>
+      <c r="I10" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Press post button on Seminar Registration List</v>
+      </c>
+      <c r="J10" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Press post button on Seminar Registration List</v>
+      </c>
+      <c r="K10" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Press post button on Seminar Registration List'</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="12">
+        <v>70</v>
+      </c>
+      <c r="I11" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Seminar registration is removed</v>
+      </c>
+      <c r="J11" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Seminar registration is removed</v>
+      </c>
+      <c r="K11" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Seminar registration is removed'</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="11" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12"/>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12" s="12">
+        <v>70</v>
+      </c>
+      <c r="I12" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Posted seminar registration exists</v>
+      </c>
+      <c r="J12" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Posted seminar registration exists</v>
+      </c>
+      <c r="K12" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Posted seminar registration exists'</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="11" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13"/>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="H13" s="12">
+        <v>70</v>
+      </c>
+      <c r="I13" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Customer related seminar ledger entry exists</v>
+      </c>
+      <c r="J13" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Customer related seminar ledger entry exists</v>
+      </c>
+      <c r="K13" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Customer related seminar ledger entry exists'</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="11" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14"/>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H14" s="12">
+        <v>70</v>
+      </c>
+      <c r="I14" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Instructor related seminar ledger entry exists</v>
+      </c>
+      <c r="J14" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Instructor related seminar ledger entry exists</v>
+      </c>
+      <c r="K14" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Instructor related seminar ledger entry exists'</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="11" customFormat="1" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15"/>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H15" s="12">
+        <v>70</v>
+      </c>
+      <c r="I15" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Room related seminar ledger entry exists</v>
+      </c>
+      <c r="J15" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Room related seminar ledger entry exists</v>
+      </c>
+      <c r="K15" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Room related seminar ledger entry exists'</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="11" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="10"/>
+      <c r="E16"/>
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="H16" s="12">
+        <v>70</v>
+      </c>
+      <c r="I16" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Instructor related resource ledger entry exists</v>
+      </c>
+      <c r="J16" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Instructor related resource ledger entry exists</v>
+      </c>
+      <c r="K16" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Instructor related resource ledger entry exists'</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="11" customFormat="1" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="10"/>
+      <c r="E17"/>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="H17" s="12">
+        <v>70</v>
+      </c>
+      <c r="I17" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Room related resource ledger entry exists</v>
+      </c>
+      <c r="J17" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Room related resource ledger entry exists</v>
+      </c>
+      <c r="K17" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Room related resource ledger entry exists' }</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="18" customFormat="1" ht="30" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G18" s="20"/>
+      <c r="H18" s="21">
+        <v>400</v>
+      </c>
+      <c r="I18" s="20" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0400] Post closed seminar registration</v>
+      </c>
+      <c r="J18" s="22" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0400] Post closed seminar registration</v>
+      </c>
+      <c r="K18" s="23" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0400 'Post closed seminar registration' {</v>
+      </c>
+      <c r="L18" s="20"/>
+    </row>
+    <row r="19" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="21">
+        <v>400</v>
+      </c>
+      <c r="I19" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Seminar</v>
+      </c>
+      <c r="J19" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Seminar</v>
+      </c>
+      <c r="K19" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Seminar'</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="H20" s="21">
+        <v>400</v>
+      </c>
+      <c r="I20" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Instructor resource</v>
+      </c>
+      <c r="J20" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Instructor resource</v>
+      </c>
+      <c r="K20" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Instructor resource'</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H21" s="21">
+        <v>400</v>
+      </c>
+      <c r="I21" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Room resource</v>
+      </c>
+      <c r="J21" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Room resource</v>
+      </c>
+      <c r="K21" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Room resource'</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="H22" s="21">
+        <v>400</v>
+      </c>
+      <c r="I22" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Customer with contact</v>
+      </c>
+      <c r="J22" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Customer with contact</v>
+      </c>
+      <c r="K22" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Customer with contact'</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H23" s="21">
+        <v>400</v>
+      </c>
+      <c r="I23" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Closed seminar registration with one participant line</v>
+      </c>
+      <c r="J23" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Closed seminar registration with one participant line</v>
+      </c>
+      <c r="K23" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Closed seminar registration with one participant line'</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H24" s="21">
+        <v>400</v>
+      </c>
+      <c r="I24" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Post seminar registration</v>
+      </c>
+      <c r="J24" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Post seminar registration</v>
+      </c>
+      <c r="K24" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Post seminar registration'</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="H25" s="21">
+        <v>400</v>
+      </c>
+      <c r="I25" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Seminar registration is removed</v>
+      </c>
+      <c r="J25" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Seminar registration is removed</v>
+      </c>
+      <c r="K25" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Seminar registration is removed'</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" s="11" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26"/>
+      <c r="F26" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="H26" s="21">
+        <v>400</v>
+      </c>
+      <c r="I26" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Posted seminar registration exists</v>
+      </c>
+      <c r="J26" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Posted seminar registration exists</v>
+      </c>
+      <c r="K26" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Posted seminar registration exists'</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" s="11" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27"/>
+      <c r="F27" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="H27" s="21">
+        <v>400</v>
+      </c>
+      <c r="I27" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Customer related seminar ledger entry exists</v>
+      </c>
+      <c r="J27" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Customer related seminar ledger entry exists</v>
+      </c>
+      <c r="K27" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Customer related seminar ledger entry exists'</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H28" s="21">
+        <v>400</v>
+      </c>
+      <c r="I28" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Instructor related seminar ledger entry exists</v>
+      </c>
+      <c r="J28" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Instructor related seminar ledger entry exists</v>
+      </c>
+      <c r="K28" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Instructor related seminar ledger entry exists'</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H29" s="21">
+        <v>400</v>
+      </c>
+      <c r="I29" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Room related seminar ledger entry exists</v>
+      </c>
+      <c r="J29" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Room related seminar ledger entry exists</v>
+      </c>
+      <c r="K29" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Room related seminar ledger entry exists'</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="H30" s="21">
+        <v>400</v>
+      </c>
+      <c r="I30" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Instructor related resource ledger entry exists</v>
+      </c>
+      <c r="J30" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Instructor related resource ledger entry exists</v>
+      </c>
+      <c r="K30" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Instructor related resource ledger entry exists'</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="H31" s="21">
+        <v>400</v>
+      </c>
+      <c r="I31" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Room related resource ledger entry exists</v>
+      </c>
+      <c r="J31" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Room related resource ledger entry exists</v>
+      </c>
+      <c r="K31" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Room related resource ledger entry exists' }</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="F32" s="18"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="21">
+        <v>401</v>
+      </c>
+      <c r="I32" s="20" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0401] Post non-closed seminar registration</v>
+      </c>
+      <c r="J32" s="22" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0401] Post non-closed seminar registration</v>
+      </c>
+      <c r="K32" s="23" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0401 'Post non-closed seminar registration' {</v>
+      </c>
+      <c r="L32" s="20"/>
+    </row>
+    <row r="33" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H33" s="12">
+        <v>401</v>
+      </c>
+      <c r="I33" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Seminar</v>
+      </c>
+      <c r="J33" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Seminar</v>
+      </c>
+      <c r="K33" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Seminar'</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" t="s">
+        <v>26</v>
+      </c>
+      <c r="F34" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="H34" s="12">
+        <v>401</v>
+      </c>
+      <c r="I34" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Instructor resource</v>
+      </c>
+      <c r="J34" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Instructor resource</v>
+      </c>
+      <c r="K34" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Instructor resource'</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" t="s">
+        <v>26</v>
+      </c>
+      <c r="F35" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H35" s="12">
+        <v>401</v>
+      </c>
+      <c r="I35" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Room resource</v>
+      </c>
+      <c r="J35" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Room resource</v>
+      </c>
+      <c r="K35" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Room resource'</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" t="s">
+        <v>26</v>
+      </c>
+      <c r="F36" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="H36" s="12">
+        <v>401</v>
+      </c>
+      <c r="I36" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Customer with contact</v>
+      </c>
+      <c r="J36" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Customer with contact</v>
+      </c>
+      <c r="K36" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Customer with contact'</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" t="s">
+        <v>26</v>
+      </c>
+      <c r="F37" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="H37" s="12">
+        <v>401</v>
+      </c>
+      <c r="I37" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Non-closed seminar registration with one participant line</v>
+      </c>
+      <c r="J37" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Non-closed seminar registration with one participant line</v>
+      </c>
+      <c r="K37" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Non-closed seminar registration with one participant line'</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H38" s="12">
+        <v>401</v>
+      </c>
+      <c r="I38" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Post seminar registration</v>
+      </c>
+      <c r="J38" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Post seminar registration</v>
+      </c>
+      <c r="K38" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Post seminar registration'</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" t="s">
+        <v>26</v>
+      </c>
+      <c r="F39" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="H39" s="12">
+        <v>401</v>
+      </c>
+      <c r="I39" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Status must be equal to closed error thrown</v>
+      </c>
+      <c r="J39" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Status must be equal to closed error thrown</v>
+      </c>
+      <c r="K39" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Status must be equal to closed error thrown' }</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="F40" s="18"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="21">
+        <v>402</v>
+      </c>
+      <c r="I40" s="20" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0402] Post closed seminar registration with empty posting date</v>
+      </c>
+      <c r="J40" s="22" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0402] Post closed seminar registration with empty posting date</v>
+      </c>
+      <c r="K40" s="23" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0402 'Post closed seminar registration with empty posting date' {</v>
+      </c>
+      <c r="L40" s="20"/>
+    </row>
+    <row r="41" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" t="s">
+        <v>26</v>
+      </c>
+      <c r="F41" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H41" s="21">
+        <v>402</v>
+      </c>
+      <c r="I41" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Seminar</v>
+      </c>
+      <c r="J41" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Seminar</v>
+      </c>
+      <c r="K41" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Seminar'</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" t="s">
+        <v>26</v>
+      </c>
+      <c r="F42" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="H42" s="21">
+        <v>402</v>
+      </c>
+      <c r="I42" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Instructor resource</v>
+      </c>
+      <c r="J42" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Instructor resource</v>
+      </c>
+      <c r="K42" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Instructor resource'</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" t="s">
+        <v>26</v>
+      </c>
+      <c r="F43" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H43" s="21">
+        <v>402</v>
+      </c>
+      <c r="I43" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Room resource</v>
+      </c>
+      <c r="J43" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Room resource</v>
+      </c>
+      <c r="K43" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Room resource'</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" t="s">
+        <v>26</v>
+      </c>
+      <c r="F44" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="H44" s="21">
+        <v>402</v>
+      </c>
+      <c r="I44" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Customer with contact</v>
+      </c>
+      <c r="J44" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Customer with contact</v>
+      </c>
+      <c r="K44" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Customer with contact'</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" t="s">
+        <v>26</v>
+      </c>
+      <c r="F45" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="H45" s="21">
+        <v>402</v>
+      </c>
+      <c r="I45" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Closed seminar registration with one participant line and empty posting date</v>
+      </c>
+      <c r="J45" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Closed seminar registration with one participant line and empty posting date</v>
+      </c>
+      <c r="K45" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Closed seminar registration with one participant line and empty posting date'</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" t="s">
+        <v>26</v>
+      </c>
+      <c r="F46" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H46" s="21">
+        <v>402</v>
+      </c>
+      <c r="I46" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Post seminar registration</v>
+      </c>
+      <c r="J46" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Post seminar registration</v>
+      </c>
+      <c r="K46" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Post seminar registration'</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47" t="s">
+        <v>26</v>
+      </c>
+      <c r="F47" t="s">
+        <v>13</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H47" s="21">
+        <v>402</v>
+      </c>
+      <c r="I47" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Posting date must be have value error thrown</v>
+      </c>
+      <c r="J47" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Posting date must be have value error thrown</v>
+      </c>
+      <c r="K47" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Posting date must be have value error thrown' }</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="F48" s="18"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="21">
+        <v>403</v>
+      </c>
+      <c r="I48" s="20" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0403] Post closed seminar registration with empty document date</v>
+      </c>
+      <c r="J48" s="22" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0403] Post closed seminar registration with empty document date</v>
+      </c>
+      <c r="K48" s="23" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0403 'Post closed seminar registration with empty document date' {</v>
+      </c>
+      <c r="L48" s="20"/>
+    </row>
+    <row r="49" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49" t="s">
+        <v>26</v>
+      </c>
+      <c r="F49" t="s">
+        <v>11</v>
+      </c>
+      <c r="G49" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H49" s="12">
+        <v>403</v>
+      </c>
+      <c r="I49" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Seminar</v>
+      </c>
+      <c r="J49" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Seminar</v>
+      </c>
+      <c r="K49" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Seminar'</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50" t="s">
+        <v>26</v>
+      </c>
+      <c r="F50" t="s">
+        <v>11</v>
+      </c>
+      <c r="G50" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="H50" s="12">
+        <v>403</v>
+      </c>
+      <c r="I50" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Instructor resource</v>
+      </c>
+      <c r="J50" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Instructor resource</v>
+      </c>
+      <c r="K50" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Instructor resource'</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>16</v>
+      </c>
+      <c r="B51" t="s">
+        <v>26</v>
+      </c>
+      <c r="F51" t="s">
+        <v>11</v>
+      </c>
+      <c r="G51" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H51" s="12">
+        <v>403</v>
+      </c>
+      <c r="I51" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Room resource</v>
+      </c>
+      <c r="J51" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Room resource</v>
+      </c>
+      <c r="K51" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Room resource'</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52" t="s">
+        <v>26</v>
+      </c>
+      <c r="F52" t="s">
+        <v>11</v>
+      </c>
+      <c r="G52" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="H52" s="12">
+        <v>403</v>
+      </c>
+      <c r="I52" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Customer with contact</v>
+      </c>
+      <c r="J52" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Customer with contact</v>
+      </c>
+      <c r="K52" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Customer with contact'</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>16</v>
+      </c>
+      <c r="B53" t="s">
+        <v>26</v>
+      </c>
+      <c r="F53" t="s">
+        <v>11</v>
+      </c>
+      <c r="G53" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="H53" s="12">
+        <v>403</v>
+      </c>
+      <c r="I53" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Closed seminar registration with one participant line and empty document date</v>
+      </c>
+      <c r="J53" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Closed seminar registration with one participant line and empty document date</v>
+      </c>
+      <c r="K53" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Closed seminar registration with one participant line and empty document date'</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>16</v>
+      </c>
+      <c r="B54" t="s">
+        <v>26</v>
+      </c>
+      <c r="F54" t="s">
+        <v>12</v>
+      </c>
+      <c r="G54" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H54" s="12">
+        <v>403</v>
+      </c>
+      <c r="I54" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Post seminar registration</v>
+      </c>
+      <c r="J54" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Post seminar registration</v>
+      </c>
+      <c r="K54" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Post seminar registration'</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>16</v>
+      </c>
+      <c r="B55" t="s">
+        <v>26</v>
+      </c>
+      <c r="F55" t="s">
+        <v>13</v>
+      </c>
+      <c r="G55" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="H55" s="12">
+        <v>403</v>
+      </c>
+      <c r="I55" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Document date must be have value error thrown</v>
+      </c>
+      <c r="J55" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Document date must be have value error thrown</v>
+      </c>
+      <c r="K55" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Document date must be have value error thrown' }</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B56" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C56" s="19"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="F56" s="18"/>
+      <c r="G56" s="20"/>
+      <c r="H56" s="21">
+        <v>404</v>
+      </c>
+      <c r="I56" s="20" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0404] Post closed seminar registration with empty seminar number</v>
+      </c>
+      <c r="J56" s="22" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0404] Post closed seminar registration with empty seminar number</v>
+      </c>
+      <c r="K56" s="23" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0404 'Post closed seminar registration with empty seminar number' {</v>
+      </c>
+      <c r="L56" s="20"/>
+    </row>
+    <row r="57" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>16</v>
+      </c>
+      <c r="B57" t="s">
+        <v>26</v>
+      </c>
+      <c r="F57" t="s">
+        <v>11</v>
+      </c>
+      <c r="G57" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H57" s="12">
+        <v>404</v>
+      </c>
+      <c r="I57" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Seminar</v>
+      </c>
+      <c r="J57" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Seminar</v>
+      </c>
+      <c r="K57" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Seminar'</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>16</v>
+      </c>
+      <c r="B58" t="s">
+        <v>26</v>
+      </c>
+      <c r="F58" t="s">
+        <v>11</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="H58" s="12">
+        <v>404</v>
+      </c>
+      <c r="I58" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Instructor resource</v>
+      </c>
+      <c r="J58" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Instructor resource</v>
+      </c>
+      <c r="K58" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Instructor resource'</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>16</v>
+      </c>
+      <c r="B59" t="s">
+        <v>26</v>
+      </c>
+      <c r="F59" t="s">
+        <v>11</v>
+      </c>
+      <c r="G59" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H59" s="12">
+        <v>404</v>
+      </c>
+      <c r="I59" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Room resource</v>
+      </c>
+      <c r="J59" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Room resource</v>
+      </c>
+      <c r="K59" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Room resource'</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>16</v>
+      </c>
+      <c r="B60" t="s">
+        <v>26</v>
+      </c>
+      <c r="F60" t="s">
+        <v>11</v>
+      </c>
+      <c r="G60" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="H60" s="12">
+        <v>404</v>
+      </c>
+      <c r="I60" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Customer with contact</v>
+      </c>
+      <c r="J60" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Customer with contact</v>
+      </c>
+      <c r="K60" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Customer with contact'</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>16</v>
+      </c>
+      <c r="B61" t="s">
+        <v>26</v>
+      </c>
+      <c r="F61" t="s">
+        <v>11</v>
+      </c>
+      <c r="G61" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="H61" s="12">
+        <v>404</v>
+      </c>
+      <c r="I61" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Closed seminar registration with one participant line and empty seminar number</v>
+      </c>
+      <c r="J61" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Closed seminar registration with one participant line and empty seminar number</v>
+      </c>
+      <c r="K61" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Closed seminar registration with one participant line and empty seminar number'</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>16</v>
+      </c>
+      <c r="B62" t="s">
+        <v>26</v>
+      </c>
+      <c r="F62" t="s">
+        <v>12</v>
+      </c>
+      <c r="G62" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H62" s="12">
+        <v>404</v>
+      </c>
+      <c r="I62" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Post seminar registration</v>
+      </c>
+      <c r="J62" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Post seminar registration</v>
+      </c>
+      <c r="K62" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Post seminar registration'</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>16</v>
+      </c>
+      <c r="B63" t="s">
+        <v>26</v>
+      </c>
+      <c r="F63" t="s">
+        <v>13</v>
+      </c>
+      <c r="G63" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="H63" s="12">
+        <v>404</v>
+      </c>
+      <c r="I63" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Seminar number must be have value error thrown</v>
+      </c>
+      <c r="J63" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Seminar number must be have value error thrown</v>
+      </c>
+      <c r="K63" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Seminar number must be have value error thrown' }</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B64" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C64" s="19"/>
+      <c r="D64" s="19"/>
+      <c r="E64" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="F64" s="18"/>
+      <c r="G64" s="20"/>
+      <c r="H64" s="21">
+        <v>405</v>
+      </c>
+      <c r="I64" s="20" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0405] Post closed seminar registration with empty duration</v>
+      </c>
+      <c r="J64" s="22" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0405] Post closed seminar registration with empty duration</v>
+      </c>
+      <c r="K64" s="23" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0405 'Post closed seminar registration with empty duration' {</v>
+      </c>
+      <c r="L64" s="20"/>
+    </row>
+    <row r="65" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>16</v>
+      </c>
+      <c r="B65" t="s">
+        <v>26</v>
+      </c>
+      <c r="F65" t="s">
+        <v>11</v>
+      </c>
+      <c r="G65" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H65" s="12">
+        <v>405</v>
+      </c>
+      <c r="I65" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Seminar</v>
+      </c>
+      <c r="J65" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Seminar</v>
+      </c>
+      <c r="K65" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Seminar'</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>16</v>
+      </c>
+      <c r="B66" t="s">
+        <v>26</v>
+      </c>
+      <c r="F66" t="s">
+        <v>11</v>
+      </c>
+      <c r="G66" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="H66" s="12">
+        <v>405</v>
+      </c>
+      <c r="I66" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Instructor resource</v>
+      </c>
+      <c r="J66" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Instructor resource</v>
+      </c>
+      <c r="K66" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Instructor resource'</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>16</v>
+      </c>
+      <c r="B67" t="s">
+        <v>26</v>
+      </c>
+      <c r="F67" t="s">
+        <v>11</v>
+      </c>
+      <c r="G67" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H67" s="12">
+        <v>405</v>
+      </c>
+      <c r="I67" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Room resource</v>
+      </c>
+      <c r="J67" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Room resource</v>
+      </c>
+      <c r="K67" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Room resource'</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>16</v>
+      </c>
+      <c r="B68" t="s">
+        <v>26</v>
+      </c>
+      <c r="F68" t="s">
+        <v>11</v>
+      </c>
+      <c r="G68" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="H68" s="12">
+        <v>405</v>
+      </c>
+      <c r="I68" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Customer with contact</v>
+      </c>
+      <c r="J68" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Customer with contact</v>
+      </c>
+      <c r="K68" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Customer with contact'</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>16</v>
+      </c>
+      <c r="B69" t="s">
+        <v>26</v>
+      </c>
+      <c r="F69" t="s">
+        <v>11</v>
+      </c>
+      <c r="G69" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="H69" s="12">
+        <v>405</v>
+      </c>
+      <c r="I69" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Closed seminar registration with one participant line and empty duration</v>
+      </c>
+      <c r="J69" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Closed seminar registration with one participant line and empty duration</v>
+      </c>
+      <c r="K69" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Closed seminar registration with one participant line and empty duration'</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>16</v>
+      </c>
+      <c r="B70" t="s">
+        <v>26</v>
+      </c>
+      <c r="F70" t="s">
+        <v>12</v>
+      </c>
+      <c r="G70" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H70" s="12">
+        <v>405</v>
+      </c>
+      <c r="I70" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Post seminar registration</v>
+      </c>
+      <c r="J70" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Post seminar registration</v>
+      </c>
+      <c r="K70" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Post seminar registration'</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>16</v>
+      </c>
+      <c r="B71" t="s">
+        <v>26</v>
+      </c>
+      <c r="F71" t="s">
+        <v>13</v>
+      </c>
+      <c r="G71" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="H71" s="12">
+        <v>405</v>
+      </c>
+      <c r="I71" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Duration must be have value error thrown</v>
+      </c>
+      <c r="J71" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Duration must be have value error thrown</v>
+      </c>
+      <c r="K71" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Duration must be have value error thrown' }</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="28.5" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B72" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C72" s="19"/>
+      <c r="D72" s="19"/>
+      <c r="E72" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="F72" s="18"/>
+      <c r="G72" s="20"/>
+      <c r="H72" s="21">
+        <v>406</v>
+      </c>
+      <c r="I72" s="20" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0406] Post closed seminar registration with empty instructor resource number</v>
+      </c>
+      <c r="J72" s="22" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0406] Post closed seminar registration with empty instructor resource number</v>
+      </c>
+      <c r="K72" s="23" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0406 'Post closed seminar registration with empty instructor resource number' {</v>
+      </c>
+      <c r="L72" s="20"/>
+    </row>
+    <row r="73" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>16</v>
+      </c>
+      <c r="B73" t="s">
+        <v>26</v>
+      </c>
+      <c r="F73" t="s">
+        <v>11</v>
+      </c>
+      <c r="G73" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H73" s="21">
+        <v>406</v>
+      </c>
+      <c r="I73" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Seminar</v>
+      </c>
+      <c r="J73" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Seminar</v>
+      </c>
+      <c r="K73" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Seminar'</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>16</v>
+      </c>
+      <c r="B74" t="s">
+        <v>26</v>
+      </c>
+      <c r="F74" t="s">
+        <v>11</v>
+      </c>
+      <c r="G74" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="H74" s="21">
+        <v>406</v>
+      </c>
+      <c r="I74" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Instructor resource</v>
+      </c>
+      <c r="J74" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Instructor resource</v>
+      </c>
+      <c r="K74" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Instructor resource'</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>16</v>
+      </c>
+      <c r="B75" t="s">
+        <v>26</v>
+      </c>
+      <c r="F75" t="s">
+        <v>11</v>
+      </c>
+      <c r="G75" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H75" s="21">
+        <v>406</v>
+      </c>
+      <c r="I75" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Room resource</v>
+      </c>
+      <c r="J75" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Room resource</v>
+      </c>
+      <c r="K75" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Room resource'</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>16</v>
+      </c>
+      <c r="B76" t="s">
+        <v>26</v>
+      </c>
+      <c r="F76" t="s">
+        <v>11</v>
+      </c>
+      <c r="G76" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="H76" s="21">
+        <v>406</v>
+      </c>
+      <c r="I76" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Customer with contact</v>
+      </c>
+      <c r="J76" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Customer with contact</v>
+      </c>
+      <c r="K76" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Customer with contact'</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>16</v>
+      </c>
+      <c r="B77" t="s">
+        <v>26</v>
+      </c>
+      <c r="F77" t="s">
+        <v>11</v>
+      </c>
+      <c r="G77" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="H77" s="21">
+        <v>406</v>
+      </c>
+      <c r="I77" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Closed seminar registration with one participant line and empty instructor resource number</v>
+      </c>
+      <c r="J77" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Closed seminar registration with one participant line and empty instructor resource number</v>
+      </c>
+      <c r="K77" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Closed seminar registration with one participant line and empty instructor resource number'</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>16</v>
+      </c>
+      <c r="B78" t="s">
+        <v>26</v>
+      </c>
+      <c r="F78" t="s">
+        <v>12</v>
+      </c>
+      <c r="G78" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H78" s="21">
+        <v>406</v>
+      </c>
+      <c r="I78" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Post seminar registration</v>
+      </c>
+      <c r="J78" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Post seminar registration</v>
+      </c>
+      <c r="K78" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Post seminar registration'</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>16</v>
+      </c>
+      <c r="B79" t="s">
+        <v>26</v>
+      </c>
+      <c r="F79" t="s">
+        <v>13</v>
+      </c>
+      <c r="G79" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H79" s="21">
+        <v>406</v>
+      </c>
+      <c r="I79" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Instructor resource number must be have value error thrown</v>
+      </c>
+      <c r="J79" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Instructor resource number must be have value error thrown</v>
+      </c>
+      <c r="K79" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Instructor resource number must be have value error thrown' }</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" ht="33" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B80" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C80" s="19"/>
+      <c r="D80" s="19"/>
+      <c r="E80" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="F80" s="18"/>
+      <c r="G80" s="20"/>
+      <c r="H80" s="21">
+        <v>407</v>
+      </c>
+      <c r="I80" s="20" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0407] Post closed seminar registration with empty room resource number</v>
+      </c>
+      <c r="J80" s="22" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0407] Post closed seminar registration with empty room resource number</v>
+      </c>
+      <c r="K80" s="23" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0407 'Post closed seminar registration with empty room resource number' {</v>
+      </c>
+      <c r="L80" s="20"/>
+    </row>
+    <row r="81" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>16</v>
+      </c>
+      <c r="B81" t="s">
+        <v>26</v>
+      </c>
+      <c r="F81" t="s">
+        <v>11</v>
+      </c>
+      <c r="G81" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H81" s="12">
+        <v>407</v>
+      </c>
+      <c r="I81" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Seminar</v>
+      </c>
+      <c r="J81" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Seminar</v>
+      </c>
+      <c r="K81" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Seminar'</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>16</v>
+      </c>
+      <c r="B82" t="s">
+        <v>26</v>
+      </c>
+      <c r="F82" t="s">
+        <v>11</v>
+      </c>
+      <c r="G82" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="H82" s="12">
+        <v>407</v>
+      </c>
+      <c r="I82" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] room resource</v>
+      </c>
+      <c r="J82" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] room resource</v>
+      </c>
+      <c r="K82" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'room resource'</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>16</v>
+      </c>
+      <c r="B83" t="s">
+        <v>26</v>
+      </c>
+      <c r="F83" t="s">
+        <v>11</v>
+      </c>
+      <c r="G83" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H83" s="12">
+        <v>407</v>
+      </c>
+      <c r="I83" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Room resource</v>
+      </c>
+      <c r="J83" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Room resource</v>
+      </c>
+      <c r="K83" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Room resource'</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>16</v>
+      </c>
+      <c r="B84" t="s">
+        <v>26</v>
+      </c>
+      <c r="F84" t="s">
+        <v>11</v>
+      </c>
+      <c r="G84" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="H84" s="12">
+        <v>407</v>
+      </c>
+      <c r="I84" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Customer with contact</v>
+      </c>
+      <c r="J84" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Customer with contact</v>
+      </c>
+      <c r="K84" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Customer with contact'</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>16</v>
+      </c>
+      <c r="B85" t="s">
+        <v>26</v>
+      </c>
+      <c r="F85" t="s">
+        <v>11</v>
+      </c>
+      <c r="G85" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="H85" s="12">
+        <v>407</v>
+      </c>
+      <c r="I85" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Closed seminar registration with one participant line and empty room resource number</v>
+      </c>
+      <c r="J85" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Closed seminar registration with one participant line and empty room resource number</v>
+      </c>
+      <c r="K85" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Closed seminar registration with one participant line and empty room resource number'</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>16</v>
+      </c>
+      <c r="B86" t="s">
+        <v>26</v>
+      </c>
+      <c r="F86" t="s">
+        <v>12</v>
+      </c>
+      <c r="G86" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H86" s="12">
+        <v>407</v>
+      </c>
+      <c r="I86" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Post seminar registration</v>
+      </c>
+      <c r="J86" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Post seminar registration</v>
+      </c>
+      <c r="K86" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Post seminar registration'</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>16</v>
+      </c>
+      <c r="B87" t="s">
+        <v>26</v>
+      </c>
+      <c r="F87" t="s">
+        <v>13</v>
+      </c>
+      <c r="G87" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H87" s="12">
+        <v>407</v>
+      </c>
+      <c r="I87" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Room resource number must be have value error thrown</v>
+      </c>
+      <c r="J87" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Room resource number must be have value error thrown</v>
+      </c>
+      <c r="K87" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Room resource number must be have value error thrown' }</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B88" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C88" s="19"/>
+      <c r="D88" s="19"/>
+      <c r="E88" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="F88" s="18"/>
+      <c r="G88" s="20"/>
+      <c r="H88" s="21">
+        <v>408</v>
+      </c>
+      <c r="I88" s="27" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0408] Post closed seminar registration with noparticipant line</v>
+      </c>
+      <c r="J88" s="28" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0408] Post closed seminar registration with noparticipant line</v>
+      </c>
+      <c r="K88" s="29" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0408 'Post closed seminar registration with noparticipant line' {</v>
+      </c>
+      <c r="L88" s="20"/>
+    </row>
+    <row r="89" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>16</v>
+      </c>
+      <c r="B89" t="s">
+        <v>26</v>
+      </c>
+      <c r="F89" t="s">
+        <v>11</v>
+      </c>
+      <c r="G89" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H89" s="12">
+        <v>408</v>
+      </c>
+      <c r="I89" s="24" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Seminar</v>
+      </c>
+      <c r="J89" s="25" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Seminar</v>
+      </c>
+      <c r="K89" s="26" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Seminar'</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>16</v>
+      </c>
+      <c r="B90" t="s">
+        <v>26</v>
+      </c>
+      <c r="F90" t="s">
+        <v>11</v>
+      </c>
+      <c r="G90" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="H90" s="12">
+        <v>408</v>
+      </c>
+      <c r="I90" s="24" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Instructor resource</v>
+      </c>
+      <c r="J90" s="25" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Instructor resource</v>
+      </c>
+      <c r="K90" s="26" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Instructor resource'</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>16</v>
+      </c>
+      <c r="B91" t="s">
+        <v>26</v>
+      </c>
+      <c r="F91" t="s">
+        <v>11</v>
+      </c>
+      <c r="G91" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H91" s="12">
+        <v>408</v>
+      </c>
+      <c r="I91" s="24" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Room resource</v>
+      </c>
+      <c r="J91" s="25" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Room resource</v>
+      </c>
+      <c r="K91" s="26" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Room resource'</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>16</v>
+      </c>
+      <c r="B92" t="s">
+        <v>26</v>
+      </c>
+      <c r="F92" t="s">
+        <v>11</v>
+      </c>
+      <c r="G92" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="H92" s="12">
+        <v>408</v>
+      </c>
+      <c r="I92" s="24" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Customer with contact</v>
+      </c>
+      <c r="J92" s="25" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Customer with contact</v>
+      </c>
+      <c r="K92" s="26" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Customer with contact'</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>16</v>
+      </c>
+      <c r="B93" t="s">
+        <v>26</v>
+      </c>
+      <c r="F93" t="s">
+        <v>11</v>
+      </c>
+      <c r="G93" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H93" s="12">
+        <v>408</v>
+      </c>
+      <c r="I93" s="24" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Closed seminar registration with no participant line</v>
+      </c>
+      <c r="J93" s="25" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Closed seminar registration with no participant line</v>
+      </c>
+      <c r="K93" s="26" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Closed seminar registration with no participant line'</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>16</v>
+      </c>
+      <c r="B94" t="s">
+        <v>26</v>
+      </c>
+      <c r="F94" t="s">
+        <v>12</v>
+      </c>
+      <c r="G94" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H94" s="12">
+        <v>408</v>
+      </c>
+      <c r="I94" s="24" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Post seminar registration</v>
+      </c>
+      <c r="J94" s="25" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Post seminar registration</v>
+      </c>
+      <c r="K94" s="26" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Post seminar registration'</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>16</v>
+      </c>
+      <c r="B95" t="s">
+        <v>26</v>
+      </c>
+      <c r="F95" t="s">
+        <v>13</v>
+      </c>
+      <c r="G95" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="H95" s="12">
+        <v>408</v>
+      </c>
+      <c r="I95" s="24" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Error thrown</v>
+      </c>
+      <c r="J95" s="25" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Error thrown</v>
+      </c>
+      <c r="K95" s="26" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Error thrown' } }</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" collapsed="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <conditionalFormatting sqref="A1:B1048576">
+    <cfRule type="containsBlanks" dxfId="11" priority="5">
+      <formula>LEN(TRIM(A1))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:D1048576">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+      <formula>"Then"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+      <formula>"Given"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26A05CD-DD6F-435A-8EFB-058B6AB8AAF4}">
-  <dimension ref="A1:L83"/>
+  <dimension ref="A1:L74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+    <sheetView topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -3223,330 +6327,34 @@
       </c>
       <c r="K73" s="14" t="str">
         <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Seminar price on line is equals seminar price on header' }</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" s="18" customFormat="1" ht="30" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B74" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C74" s="19"/>
-      <c r="D74" s="19"/>
-      <c r="E74" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="G74" s="20"/>
-      <c r="H74" s="21">
-        <v>70</v>
-      </c>
-      <c r="I74" s="29" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0070] Post seminar registration from Seminar Registration List page</v>
-      </c>
-      <c r="J74" s="30" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0070] Post seminar registration from Seminar Registration List page</v>
-      </c>
-      <c r="K74" s="31" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0070 'Post seminar registration from Seminar Registration List page' {</v>
-      </c>
-      <c r="L74" s="20"/>
-    </row>
-    <row r="75" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>16</v>
-      </c>
-      <c r="B75" t="s">
-        <v>26</v>
-      </c>
-      <c r="E75" s="24"/>
-      <c r="F75" t="s">
-        <v>11</v>
-      </c>
-      <c r="G75" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H75" s="12">
-        <v>70</v>
-      </c>
-      <c r="I75" s="25" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Seminar</v>
-      </c>
-      <c r="J75" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Seminar</v>
-      </c>
-      <c r="K75" s="27" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Seminar'</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>16</v>
-      </c>
-      <c r="B76" t="s">
-        <v>26</v>
-      </c>
-      <c r="E76" s="24"/>
-      <c r="F76" t="s">
-        <v>11</v>
-      </c>
-      <c r="G76" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="H76" s="12">
-        <v>70</v>
-      </c>
-      <c r="I76" s="25" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Instructor resource</v>
-      </c>
-      <c r="J76" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Instructor resource</v>
-      </c>
-      <c r="K76" s="27" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Instructor resource'</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>16</v>
-      </c>
-      <c r="B77" t="s">
-        <v>26</v>
-      </c>
-      <c r="E77" s="24"/>
-      <c r="F77" t="s">
-        <v>11</v>
-      </c>
-      <c r="G77" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="H77" s="12">
-        <v>70</v>
-      </c>
-      <c r="I77" s="25" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Room resource</v>
-      </c>
-      <c r="J77" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Room resource</v>
-      </c>
-      <c r="K77" s="27" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Room resource'</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>16</v>
-      </c>
-      <c r="B78" t="s">
-        <v>26</v>
-      </c>
-      <c r="E78" s="24"/>
-      <c r="F78" t="s">
-        <v>11</v>
-      </c>
-      <c r="G78" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="H78" s="12">
-        <v>70</v>
-      </c>
-      <c r="I78" s="25" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Closed seminar registration with  one participant line</v>
-      </c>
-      <c r="J78" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Closed seminar registration with  one participant line</v>
-      </c>
-      <c r="K78" s="27" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Closed seminar registration with  one participant line'</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>16</v>
-      </c>
-      <c r="B79" t="s">
-        <v>26</v>
-      </c>
-      <c r="E79" s="24"/>
-      <c r="F79" t="s">
-        <v>12</v>
-      </c>
-      <c r="G79" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="H79" s="12">
-        <v>70</v>
-      </c>
-      <c r="I79" s="25" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Press post button on Seminar Registration List</v>
-      </c>
-      <c r="J79" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Press post button on Seminar Registration List</v>
-      </c>
-      <c r="K79" s="27" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Press post button on Seminar Registration List'</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>16</v>
-      </c>
-      <c r="B80" t="s">
-        <v>26</v>
-      </c>
-      <c r="E80" s="24"/>
-      <c r="F80" t="s">
-        <v>13</v>
-      </c>
-      <c r="G80" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="H80" s="12">
-        <v>70</v>
-      </c>
-      <c r="I80" s="25" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Seminar registration is removed</v>
-      </c>
-      <c r="J80" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Seminar registration is removed</v>
-      </c>
-      <c r="K80" s="27" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Seminar registration is removed'</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>16</v>
-      </c>
-      <c r="B81" t="s">
-        <v>26</v>
-      </c>
-      <c r="E81" s="24"/>
-      <c r="F81" t="s">
-        <v>13</v>
-      </c>
-      <c r="G81" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="H81" s="12">
-        <v>70</v>
-      </c>
-      <c r="I81" s="25" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Posted seminar registration exists</v>
-      </c>
-      <c r="J81" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Posted seminar registration exists</v>
-      </c>
-      <c r="K81" s="27" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Posted seminar registration exists'</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>16</v>
-      </c>
-      <c r="B82" t="s">
-        <v>26</v>
-      </c>
-      <c r="E82" s="24"/>
-      <c r="F82" t="s">
-        <v>13</v>
-      </c>
-      <c r="G82" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="H82" s="12">
-        <v>70</v>
-      </c>
-      <c r="I82" s="25" t="str">
-        <f>IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table29[[#This Row],[Feature]]," ",Table29[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table29[[#This Row],[Scenario '#]],"0000"),"] ",Table29[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table29[[#This Row],[Given-When-Then (Tag)]]),"] ",Table29[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Related ledger entries exist</v>
-      </c>
-      <c r="J82" s="26" t="str">
-        <f>_xlfn.CONCAT("//",Table29[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Related ledger entries exist</v>
-      </c>
-      <c r="K82" s="27" t="str">
-        <f ca="1">IF(Table29[[#This Row],[Given-When-Then (Tag)]]="",IF(Table29[[#This Row],[Scenario]]="",IF(Table29[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table29[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table29[[#This Row],[Scenario '#]],"0000")," '",Table29[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table29[[#This Row],[Given-When-Then (Tag)]]," '",Table29[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Related ledger entries exist' } }</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" collapsed="1" x14ac:dyDescent="0.25"/>
+        <v>Then 'Seminar price on line is equals seminar price on header' } }</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" collapsed="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="A1:B29">
-    <cfRule type="containsBlanks" dxfId="11" priority="5">
+  <conditionalFormatting sqref="A1:B1048576">
+    <cfRule type="containsBlanks" dxfId="5" priority="5">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A30:B1048576">
-    <cfRule type="containsBlanks" dxfId="10" priority="33">
-      <formula>LEN(TRIM(A30))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1:D29">
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+  <conditionalFormatting sqref="C1:D1048576">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30:D1048576">
-    <cfRule type="cellIs" dxfId="8" priority="35" operator="equal">
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D29">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D30:D1048576">
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
-      <formula>"X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F53">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Then"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
-      <formula>"Given"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F54:F1048576">
-    <cfRule type="cellIs" dxfId="2" priority="20" operator="equal">
-      <formula>"Then"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="21" operator="equal">
-      <formula>"When"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"Given"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Set up different technical versions of the tests
</commit_message>
<xml_diff>
--- a/test/atdd scenarios/Seminar Registration - ATDD Scenarios.xlsx
+++ b/test/atdd scenarios/Seminar Registration - ATDD Scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2a63c87061b9b9b/Presentations/DOK/2024/Nordic/Presentation 1 - Tip ^0 Tricks for efficient and effective test automation data setup/Code Examples/Seminar Management/test/atdd scenarios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="230" documentId="13_ncr:1_{BB4C36B7-EE5C-4F78-9FD6-35C3B4ED61F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90CB6D44-EB5C-4656-99CF-E41CBBE6A390}"/>
+  <xr:revisionPtr revIDLastSave="259" documentId="13_ncr:1_{BB4C36B7-EE5C-4F78-9FD6-35C3B4ED61F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D5271BF-BFB7-45A0-A436-D15EF75657A2}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27720" windowHeight="16440" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios - Posting only" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="122">
   <si>
     <t>Feature</t>
   </si>
@@ -388,9 +388,6 @@
     <t>Post closed seminar registration with empty room resource number</t>
   </si>
   <si>
-    <t>room resource</t>
-  </si>
-  <si>
     <t>Closed seminar registration with one participant line and empty room resource number</t>
   </si>
   <si>
@@ -400,10 +397,10 @@
     <t>Closed seminar registration with no participant line</t>
   </si>
   <si>
-    <t>Post closed seminar registration with noparticipant line</t>
-  </si>
-  <si>
     <t>Error thrown</t>
+  </si>
+  <si>
+    <t>Post closed seminar registration with no participant line</t>
   </si>
 </sst>
 </file>
@@ -496,7 +493,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -561,24 +558,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -823,8 +802,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{22F2C4D7-A7F8-46C0-960F-675A8BCE1D8D}" name="Table293" displayName="Table293" ref="A1:L95" totalsRowShown="0" headerRowDxfId="31">
-  <autoFilter ref="A1:L95" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{22F2C4D7-A7F8-46C0-960F-675A8BCE1D8D}" name="Table293" displayName="Table293" ref="A1:L94" totalsRowShown="0" headerRowDxfId="31">
+  <autoFilter ref="A1:L94" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{3C5A203A-70AF-48EA-9EC7-2C4C4E6D6F0C}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{B34F943B-2E52-4D5D-96D0-D87B15881916}" name="Sub Feature"/>
@@ -1173,9 +1152,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7684FF22-50C0-48D3-B42F-054142E19464}">
-  <dimension ref="A1:L96"/>
+  <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G92" sqref="G92"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3639,22 +3620,22 @@
         <v>11</v>
       </c>
       <c r="G82" s="11" t="s">
-        <v>117</v>
+        <v>81</v>
       </c>
       <c r="H82" s="12">
         <v>407</v>
       </c>
       <c r="I82" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] room resource</v>
+        <v>[GIVEN] Instructor resource</v>
       </c>
       <c r="J82" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] room resource</v>
+        <v>//[GIVEN] Instructor resource</v>
       </c>
       <c r="K82" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'room resource'</v>
+        <v>Given 'Instructor resource'</v>
       </c>
     </row>
     <row r="83" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3726,7 +3707,7 @@
         <v>11</v>
       </c>
       <c r="G85" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H85" s="12">
         <v>407</v>
@@ -3784,7 +3765,7 @@
         <v>13</v>
       </c>
       <c r="G87" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H87" s="12">
         <v>407</v>
@@ -3819,17 +3800,17 @@
       <c r="H88" s="21">
         <v>408</v>
       </c>
-      <c r="I88" s="27" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0408] Post closed seminar registration with noparticipant line</v>
-      </c>
-      <c r="J88" s="28" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0408] Post closed seminar registration with noparticipant line</v>
-      </c>
-      <c r="K88" s="29" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0408 'Post closed seminar registration with noparticipant line' {</v>
+      <c r="I88" s="20" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0408] Post closed seminar registration with no participant line</v>
+      </c>
+      <c r="J88" s="22" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0408] Post closed seminar registration with no participant line</v>
+      </c>
+      <c r="K88" s="23" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0408 'Post closed seminar registration with no participant line' {</v>
       </c>
       <c r="L88" s="20"/>
     </row>
@@ -3849,15 +3830,15 @@
       <c r="H89" s="12">
         <v>408</v>
       </c>
-      <c r="I89" s="24" t="str">
+      <c r="I89" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[GIVEN] Seminar</v>
       </c>
-      <c r="J89" s="25" t="str">
+      <c r="J89" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Seminar</v>
       </c>
-      <c r="K89" s="26" t="str">
+      <c r="K89" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Given 'Seminar'</v>
       </c>
@@ -3878,15 +3859,15 @@
       <c r="H90" s="12">
         <v>408</v>
       </c>
-      <c r="I90" s="24" t="str">
+      <c r="I90" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[GIVEN] Instructor resource</v>
       </c>
-      <c r="J90" s="25" t="str">
+      <c r="J90" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Instructor resource</v>
       </c>
-      <c r="K90" s="26" t="str">
+      <c r="K90" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Given 'Instructor resource'</v>
       </c>
@@ -3907,20 +3888,20 @@
       <c r="H91" s="12">
         <v>408</v>
       </c>
-      <c r="I91" s="24" t="str">
+      <c r="I91" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[GIVEN] Room resource</v>
       </c>
-      <c r="J91" s="25" t="str">
+      <c r="J91" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Room resource</v>
       </c>
-      <c r="K91" s="26" t="str">
+      <c r="K91" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Given 'Room resource'</v>
       </c>
     </row>
-    <row r="92" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>16</v>
       </c>
@@ -3931,25 +3912,25 @@
         <v>11</v>
       </c>
       <c r="G92" s="11" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="H92" s="12">
         <v>408</v>
       </c>
-      <c r="I92" s="24" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Customer with contact</v>
-      </c>
-      <c r="J92" s="25" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Customer with contact</v>
-      </c>
-      <c r="K92" s="26" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Customer with contact'</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="I92" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Closed seminar registration with no participant line</v>
+      </c>
+      <c r="J92" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Closed seminar registration with no participant line</v>
+      </c>
+      <c r="K92" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Closed seminar registration with no participant line'</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>16</v>
       </c>
@@ -3957,25 +3938,25 @@
         <v>26</v>
       </c>
       <c r="F93" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G93" s="11" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="H93" s="12">
         <v>408</v>
       </c>
-      <c r="I93" s="24" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Closed seminar registration with no participant line</v>
-      </c>
-      <c r="J93" s="25" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Closed seminar registration with no participant line</v>
-      </c>
-      <c r="K93" s="26" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Closed seminar registration with no participant line'</v>
+      <c r="I93" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Post seminar registration</v>
+      </c>
+      <c r="J93" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Post seminar registration</v>
+      </c>
+      <c r="K93" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Post seminar registration'</v>
       </c>
     </row>
     <row r="94" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3986,57 +3967,28 @@
         <v>26</v>
       </c>
       <c r="F94" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G94" s="11" t="s">
-        <v>86</v>
+        <v>120</v>
       </c>
       <c r="H94" s="12">
         <v>408</v>
       </c>
-      <c r="I94" s="24" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Post seminar registration</v>
-      </c>
-      <c r="J94" s="25" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Post seminar registration</v>
-      </c>
-      <c r="K94" s="26" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Post seminar registration'</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>16</v>
-      </c>
-      <c r="B95" t="s">
-        <v>26</v>
-      </c>
-      <c r="F95" t="s">
-        <v>13</v>
-      </c>
-      <c r="G95" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="H95" s="12">
-        <v>408</v>
-      </c>
-      <c r="I95" s="24" t="str">
+      <c r="I94" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[THEN] Error thrown</v>
       </c>
-      <c r="J95" s="25" t="str">
+      <c r="J94" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
         <v>//[THEN] Error thrown</v>
       </c>
-      <c r="K95" s="26" t="str">
+      <c r="K94" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Then 'Error thrown' } }</v>
       </c>
     </row>
-    <row r="96" spans="1:12" collapsed="1" x14ac:dyDescent="0.25"/>
+    <row r="95" spans="1:12" collapsed="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="A1:B1048576">
     <cfRule type="containsBlanks" dxfId="11" priority="5">

</xml_diff>

<commit_message>
Added comment to each test codeunit to explain it's scope and updated ATDD sheet
</commit_message>
<xml_diff>
--- a/test/atdd scenarios/Seminar Registration - ATDD Scenarios.xlsx
+++ b/test/atdd scenarios/Seminar Registration - ATDD Scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2a63c87061b9b9b/Presentations/DOK/2024/Nordic/Presentation 1 - Tip ^0 Tricks for efficient and effective test automation data setup/Code Examples/Seminar Management/test/atdd scenarios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="259" documentId="13_ncr:1_{BB4C36B7-EE5C-4F78-9FD6-35C3B4ED61F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D5271BF-BFB7-45A0-A436-D15EF75657A2}"/>
+  <xr:revisionPtr revIDLastSave="285" documentId="13_ncr:1_{BB4C36B7-EE5C-4F78-9FD6-35C3B4ED61F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48A0C659-17BD-4C7B-AA7C-A3CA8FCA84A8}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="675" yWindow="1140" windowWidth="21600" windowHeight="11385" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
+    <workbookView xWindow="-25320" yWindow="285" windowWidth="24120" windowHeight="15990" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios - Posting only" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="122">
   <si>
     <t>Feature</t>
   </si>
@@ -1154,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7684FF22-50C0-48D3-B42F-054142E19464}">
   <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G92" sqref="G92"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33:D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -2153,7 +2153,9 @@
         <v>26</v>
       </c>
       <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
+      <c r="D32" s="19" t="s">
+        <v>14</v>
+      </c>
       <c r="E32" s="18" t="s">
         <v>97</v>
       </c>
@@ -2183,6 +2185,9 @@
       <c r="B33" t="s">
         <v>26</v>
       </c>
+      <c r="D33" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F33" t="s">
         <v>11</v>
       </c>
@@ -2212,6 +2217,9 @@
       <c r="B34" t="s">
         <v>26</v>
       </c>
+      <c r="D34" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F34" t="s">
         <v>11</v>
       </c>
@@ -2241,6 +2249,9 @@
       <c r="B35" t="s">
         <v>26</v>
       </c>
+      <c r="D35" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F35" t="s">
         <v>11</v>
       </c>
@@ -2270,6 +2281,9 @@
       <c r="B36" t="s">
         <v>26</v>
       </c>
+      <c r="D36" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F36" t="s">
         <v>11</v>
       </c>
@@ -2299,6 +2313,9 @@
       <c r="B37" t="s">
         <v>26</v>
       </c>
+      <c r="D37" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F37" t="s">
         <v>11</v>
       </c>
@@ -2328,6 +2345,9 @@
       <c r="B38" t="s">
         <v>26</v>
       </c>
+      <c r="D38" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F38" t="s">
         <v>12</v>
       </c>
@@ -2357,6 +2377,9 @@
       <c r="B39" t="s">
         <v>26</v>
       </c>
+      <c r="D39" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F39" t="s">
         <v>13</v>
       </c>
@@ -2387,7 +2410,9 @@
         <v>26</v>
       </c>
       <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
+      <c r="D40" s="19" t="s">
+        <v>14</v>
+      </c>
       <c r="E40" s="18" t="s">
         <v>99</v>
       </c>
@@ -2417,6 +2442,9 @@
       <c r="B41" t="s">
         <v>26</v>
       </c>
+      <c r="D41" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F41" t="s">
         <v>11</v>
       </c>
@@ -2446,6 +2474,9 @@
       <c r="B42" t="s">
         <v>26</v>
       </c>
+      <c r="D42" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F42" t="s">
         <v>11</v>
       </c>
@@ -2475,6 +2506,9 @@
       <c r="B43" t="s">
         <v>26</v>
       </c>
+      <c r="D43" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F43" t="s">
         <v>11</v>
       </c>
@@ -2504,6 +2538,9 @@
       <c r="B44" t="s">
         <v>26</v>
       </c>
+      <c r="D44" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F44" t="s">
         <v>11</v>
       </c>
@@ -2533,6 +2570,9 @@
       <c r="B45" t="s">
         <v>26</v>
       </c>
+      <c r="D45" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F45" t="s">
         <v>11</v>
       </c>
@@ -2562,6 +2602,9 @@
       <c r="B46" t="s">
         <v>26</v>
       </c>
+      <c r="D46" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F46" t="s">
         <v>12</v>
       </c>
@@ -2591,6 +2634,9 @@
       <c r="B47" t="s">
         <v>26</v>
       </c>
+      <c r="D47" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F47" t="s">
         <v>13</v>
       </c>
@@ -2621,7 +2667,9 @@
         <v>26</v>
       </c>
       <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
+      <c r="D48" s="19" t="s">
+        <v>14</v>
+      </c>
       <c r="E48" s="18" t="s">
         <v>104</v>
       </c>
@@ -2651,6 +2699,9 @@
       <c r="B49" t="s">
         <v>26</v>
       </c>
+      <c r="D49" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F49" t="s">
         <v>11</v>
       </c>
@@ -2680,6 +2731,9 @@
       <c r="B50" t="s">
         <v>26</v>
       </c>
+      <c r="D50" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F50" t="s">
         <v>11</v>
       </c>
@@ -2709,6 +2763,9 @@
       <c r="B51" t="s">
         <v>26</v>
       </c>
+      <c r="D51" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F51" t="s">
         <v>11</v>
       </c>
@@ -2738,6 +2795,9 @@
       <c r="B52" t="s">
         <v>26</v>
       </c>
+      <c r="D52" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F52" t="s">
         <v>11</v>
       </c>
@@ -2767,6 +2827,9 @@
       <c r="B53" t="s">
         <v>26</v>
       </c>
+      <c r="D53" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F53" t="s">
         <v>11</v>
       </c>
@@ -2796,6 +2859,9 @@
       <c r="B54" t="s">
         <v>26</v>
       </c>
+      <c r="D54" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F54" t="s">
         <v>12</v>
       </c>
@@ -2825,6 +2891,9 @@
       <c r="B55" t="s">
         <v>26</v>
       </c>
+      <c r="D55" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F55" t="s">
         <v>13</v>
       </c>
@@ -2855,7 +2924,9 @@
         <v>26</v>
       </c>
       <c r="C56" s="19"/>
-      <c r="D56" s="19"/>
+      <c r="D56" s="19" t="s">
+        <v>14</v>
+      </c>
       <c r="E56" s="18" t="s">
         <v>107</v>
       </c>
@@ -2885,6 +2956,9 @@
       <c r="B57" t="s">
         <v>26</v>
       </c>
+      <c r="D57" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F57" t="s">
         <v>11</v>
       </c>
@@ -2914,6 +2988,9 @@
       <c r="B58" t="s">
         <v>26</v>
       </c>
+      <c r="D58" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F58" t="s">
         <v>11</v>
       </c>
@@ -2943,6 +3020,9 @@
       <c r="B59" t="s">
         <v>26</v>
       </c>
+      <c r="D59" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F59" t="s">
         <v>11</v>
       </c>
@@ -2972,6 +3052,9 @@
       <c r="B60" t="s">
         <v>26</v>
       </c>
+      <c r="D60" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F60" t="s">
         <v>11</v>
       </c>
@@ -3001,6 +3084,9 @@
       <c r="B61" t="s">
         <v>26</v>
       </c>
+      <c r="D61" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F61" t="s">
         <v>11</v>
       </c>
@@ -3030,6 +3116,9 @@
       <c r="B62" t="s">
         <v>26</v>
       </c>
+      <c r="D62" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F62" t="s">
         <v>12</v>
       </c>
@@ -3059,6 +3148,9 @@
       <c r="B63" t="s">
         <v>26</v>
       </c>
+      <c r="D63" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F63" t="s">
         <v>13</v>
       </c>
@@ -3089,7 +3181,9 @@
         <v>26</v>
       </c>
       <c r="C64" s="19"/>
-      <c r="D64" s="19"/>
+      <c r="D64" s="19" t="s">
+        <v>14</v>
+      </c>
       <c r="E64" s="18" t="s">
         <v>110</v>
       </c>
@@ -3119,6 +3213,9 @@
       <c r="B65" t="s">
         <v>26</v>
       </c>
+      <c r="D65" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F65" t="s">
         <v>11</v>
       </c>
@@ -3148,6 +3245,9 @@
       <c r="B66" t="s">
         <v>26</v>
       </c>
+      <c r="D66" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F66" t="s">
         <v>11</v>
       </c>
@@ -3177,6 +3277,9 @@
       <c r="B67" t="s">
         <v>26</v>
       </c>
+      <c r="D67" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F67" t="s">
         <v>11</v>
       </c>
@@ -3206,6 +3309,9 @@
       <c r="B68" t="s">
         <v>26</v>
       </c>
+      <c r="D68" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F68" t="s">
         <v>11</v>
       </c>
@@ -3235,6 +3341,9 @@
       <c r="B69" t="s">
         <v>26</v>
       </c>
+      <c r="D69" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F69" t="s">
         <v>11</v>
       </c>
@@ -3264,6 +3373,9 @@
       <c r="B70" t="s">
         <v>26</v>
       </c>
+      <c r="D70" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F70" t="s">
         <v>12</v>
       </c>
@@ -3293,6 +3405,9 @@
       <c r="B71" t="s">
         <v>26</v>
       </c>
+      <c r="D71" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F71" t="s">
         <v>13</v>
       </c>
@@ -3323,7 +3438,9 @@
         <v>26</v>
       </c>
       <c r="C72" s="19"/>
-      <c r="D72" s="19"/>
+      <c r="D72" s="19" t="s">
+        <v>14</v>
+      </c>
       <c r="E72" s="18" t="s">
         <v>113</v>
       </c>
@@ -3353,6 +3470,9 @@
       <c r="B73" t="s">
         <v>26</v>
       </c>
+      <c r="D73" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F73" t="s">
         <v>11</v>
       </c>
@@ -3382,6 +3502,9 @@
       <c r="B74" t="s">
         <v>26</v>
       </c>
+      <c r="D74" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F74" t="s">
         <v>11</v>
       </c>
@@ -3411,6 +3534,9 @@
       <c r="B75" t="s">
         <v>26</v>
       </c>
+      <c r="D75" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F75" t="s">
         <v>11</v>
       </c>
@@ -3440,6 +3566,9 @@
       <c r="B76" t="s">
         <v>26</v>
       </c>
+      <c r="D76" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F76" t="s">
         <v>11</v>
       </c>
@@ -3469,6 +3598,9 @@
       <c r="B77" t="s">
         <v>26</v>
       </c>
+      <c r="D77" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F77" t="s">
         <v>11</v>
       </c>
@@ -3498,6 +3630,9 @@
       <c r="B78" t="s">
         <v>26</v>
       </c>
+      <c r="D78" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F78" t="s">
         <v>12</v>
       </c>
@@ -3527,6 +3662,9 @@
       <c r="B79" t="s">
         <v>26</v>
       </c>
+      <c r="D79" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F79" t="s">
         <v>13</v>
       </c>
@@ -3557,7 +3695,9 @@
         <v>26</v>
       </c>
       <c r="C80" s="19"/>
-      <c r="D80" s="19"/>
+      <c r="D80" s="19" t="s">
+        <v>14</v>
+      </c>
       <c r="E80" s="18" t="s">
         <v>116</v>
       </c>
@@ -3587,6 +3727,9 @@
       <c r="B81" t="s">
         <v>26</v>
       </c>
+      <c r="D81" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F81" t="s">
         <v>11</v>
       </c>
@@ -3616,6 +3759,9 @@
       <c r="B82" t="s">
         <v>26</v>
       </c>
+      <c r="D82" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F82" t="s">
         <v>11</v>
       </c>
@@ -3645,6 +3791,9 @@
       <c r="B83" t="s">
         <v>26</v>
       </c>
+      <c r="D83" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F83" t="s">
         <v>11</v>
       </c>
@@ -3674,6 +3823,9 @@
       <c r="B84" t="s">
         <v>26</v>
       </c>
+      <c r="D84" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F84" t="s">
         <v>11</v>
       </c>
@@ -3703,6 +3855,9 @@
       <c r="B85" t="s">
         <v>26</v>
       </c>
+      <c r="D85" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F85" t="s">
         <v>11</v>
       </c>
@@ -3732,6 +3887,9 @@
       <c r="B86" t="s">
         <v>26</v>
       </c>
+      <c r="D86" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F86" t="s">
         <v>12</v>
       </c>
@@ -3761,6 +3919,9 @@
       <c r="B87" t="s">
         <v>26</v>
       </c>
+      <c r="D87" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F87" t="s">
         <v>13</v>
       </c>
@@ -3791,7 +3952,9 @@
         <v>26</v>
       </c>
       <c r="C88" s="19"/>
-      <c r="D88" s="19"/>
+      <c r="D88" s="19" t="s">
+        <v>14</v>
+      </c>
       <c r="E88" s="18" t="s">
         <v>121</v>
       </c>
@@ -3821,6 +3984,9 @@
       <c r="B89" t="s">
         <v>26</v>
       </c>
+      <c r="D89" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F89" t="s">
         <v>11</v>
       </c>
@@ -3850,6 +4016,9 @@
       <c r="B90" t="s">
         <v>26</v>
       </c>
+      <c r="D90" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F90" t="s">
         <v>11</v>
       </c>
@@ -3879,6 +4048,9 @@
       <c r="B91" t="s">
         <v>26</v>
       </c>
+      <c r="D91" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F91" t="s">
         <v>11</v>
       </c>
@@ -3908,6 +4080,9 @@
       <c r="B92" t="s">
         <v>26</v>
       </c>
+      <c r="D92" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F92" t="s">
         <v>11</v>
       </c>
@@ -3937,6 +4112,9 @@
       <c r="B93" t="s">
         <v>26</v>
       </c>
+      <c r="D93" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F93" t="s">
         <v>12</v>
       </c>
@@ -3965,6 +4143,9 @@
       </c>
       <c r="B94" t="s">
         <v>26</v>
+      </c>
+      <c r="D94" s="10" t="s">
+        <v>14</v>
       </c>
       <c r="F94" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Update to BC24 and fixed some typos
</commit_message>
<xml_diff>
--- a/test/atdd scenarios/Seminar Registration - ATDD Scenarios.xlsx
+++ b/test/atdd scenarios/Seminar Registration - ATDD Scenarios.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2a63c87061b9b9b/Presentations/DOK/2024/Nordic/Presentation 1 - Tip ^0 Tricks for efficient and effective test automation data setup/Code Examples/Seminar Management/test/atdd scenarios/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2a63c87061b9b9b/Presentations/DOK/2024/Nordic/Presentation 1 - Tips ^0 Tricks for efficient and effective test automation data setup/Code Examples/Seminar Management/test/atdd scenarios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="285" documentId="13_ncr:1_{BB4C36B7-EE5C-4F78-9FD6-35C3B4ED61F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48A0C659-17BD-4C7B-AA7C-A3CA8FCA84A8}"/>
+  <xr:revisionPtr revIDLastSave="290" documentId="13_ncr:1_{BB4C36B7-EE5C-4F78-9FD6-35C3B4ED61F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8196EA7-DD66-4689-9153-60A5C0EE04B6}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="285" windowWidth="24120" windowHeight="15990" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios - Posting only" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="124">
   <si>
     <t>Feature</t>
   </si>
@@ -401,6 +401,12 @@
   </si>
   <si>
     <t>Post closed seminar registration with no participant line</t>
+  </si>
+  <si>
+    <t>Bill-to Customer empty</t>
+  </si>
+  <si>
+    <t>Participant empty</t>
   </si>
 </sst>
 </file>
@@ -802,8 +808,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{22F2C4D7-A7F8-46C0-960F-675A8BCE1D8D}" name="Table293" displayName="Table293" ref="A1:L94" totalsRowShown="0" headerRowDxfId="31">
-  <autoFilter ref="A1:L94" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{22F2C4D7-A7F8-46C0-960F-675A8BCE1D8D}" name="Table293" displayName="Table293" ref="A1:L96" totalsRowShown="0" headerRowDxfId="31">
+  <autoFilter ref="A1:L96" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{3C5A203A-70AF-48EA-9EC7-2C4C4E6D6F0C}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{B34F943B-2E52-4D5D-96D0-D87B15881916}" name="Sub Feature"/>
@@ -1152,10 +1158,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7684FF22-50C0-48D3-B42F-054142E19464}">
-  <dimension ref="A1:L95"/>
+  <dimension ref="A1:L96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33:D39"/>
+      <selection activeCell="E97" sqref="E97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -4166,10 +4172,43 @@
       </c>
       <c r="K94" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Error thrown' } }</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" collapsed="1" x14ac:dyDescent="0.25"/>
+        <v>Then 'Error thrown' }</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="E95" t="s">
+        <v>122</v>
+      </c>
+      <c r="I95" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0000] Bill-to Customer empty</v>
+      </c>
+      <c r="J95" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0000] Bill-to Customer empty</v>
+      </c>
+      <c r="K95" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0000 'Bill-to Customer empty' {</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E96" t="s">
+        <v>123</v>
+      </c>
+      <c r="I96" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0000] Participant empty</v>
+      </c>
+      <c r="J96" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0000] Participant empty</v>
+      </c>
+      <c r="K96" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0000 'Participant empty' {</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:B1048576">
     <cfRule type="containsBlanks" dxfId="11" priority="5">

</xml_diff>

<commit_message>
Added tests for empty Bill-to Customer No. and empty Participant Contact No. fields
</commit_message>
<xml_diff>
--- a/test/atdd scenarios/Seminar Registration - ATDD Scenarios.xlsx
+++ b/test/atdd scenarios/Seminar Registration - ATDD Scenarios.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2a63c87061b9b9b/Presentations/DOK/2024/Nordic/Presentation 1 - Tips ^0 Tricks for efficient and effective test automation data setup/Code Examples/Seminar Management/test/atdd scenarios/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\OneDrive\Presentations\DOK\2024\Nordic\Presentation 1 - Tips &amp; Tricks for efficient and effective test automation data setup\Code Examples\Seminar Management\test\atdd scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="290" documentId="13_ncr:1_{BB4C36B7-EE5C-4F78-9FD6-35C3B4ED61F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8196EA7-DD66-4689-9153-60A5C0EE04B6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1643C2B1-EA4C-4D1D-97AA-B1BFC59B4C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27720" windowHeight="16440" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
   <sheets>
     <sheet name="ATDD Scenarios - Posting only" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="125">
   <si>
     <t>Feature</t>
   </si>
@@ -298,9 +298,6 @@
     <t>Post seminar registration</t>
   </si>
   <si>
-    <t>Customer with contact</t>
-  </si>
-  <si>
     <t>Room related seminar ledger entry exists</t>
   </si>
   <si>
@@ -403,10 +400,16 @@
     <t>Post closed seminar registration with no participant line</t>
   </si>
   <si>
-    <t>Bill-to Customer empty</t>
-  </si>
-  <si>
-    <t>Participant empty</t>
+    <t>Post closed seminar registration with participant line with empty bill-to customer number</t>
+  </si>
+  <si>
+    <t>Post closed seminar registration with participant line with empty participant number</t>
+  </si>
+  <si>
+    <t>Closed seminar registration with one participant line with empty bill-to customer number</t>
+  </si>
+  <si>
+    <t>Closed seminar registration with one participant line with empty participant number</t>
   </si>
 </sst>
 </file>
@@ -499,7 +502,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -564,6 +567,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -808,8 +821,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{22F2C4D7-A7F8-46C0-960F-675A8BCE1D8D}" name="Table293" displayName="Table293" ref="A1:L96" totalsRowShown="0" headerRowDxfId="31">
-  <autoFilter ref="A1:L96" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{22F2C4D7-A7F8-46C0-960F-675A8BCE1D8D}" name="Table293" displayName="Table293" ref="A1:L117" totalsRowShown="0" headerRowDxfId="31">
+  <autoFilter ref="A1:L117" xr:uid="{74C06549-5BDA-49EA-8217-9DE86359CCAF}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{3C5A203A-70AF-48EA-9EC7-2C4C4E6D6F0C}" name="Feature"/>
     <tableColumn id="9" xr3:uid="{B34F943B-2E52-4D5D-96D0-D87B15881916}" name="Sub Feature"/>
@@ -1158,11 +1171,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7684FF22-50C0-48D3-B42F-054142E19464}">
-  <dimension ref="A1:L96"/>
+  <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E97" sqref="E97"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1258,7 +1269,7 @@
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G3" s="20"/>
       <c r="H3" s="21">
@@ -1388,7 +1399,7 @@
         <v>11</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H7" s="12">
         <v>70</v>
@@ -1420,7 +1431,7 @@
         <v>11</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H8" s="12">
         <v>70</v>
@@ -1452,7 +1463,7 @@
         <v>11</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H9" s="12">
         <v>70</v>
@@ -1584,7 +1595,7 @@
         <v>13</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H13" s="12">
         <v>70</v>
@@ -1618,7 +1629,7 @@
         <v>13</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H14" s="12">
         <v>70</v>
@@ -1652,7 +1663,7 @@
         <v>13</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H15" s="12">
         <v>70</v>
@@ -1686,7 +1697,7 @@
         <v>13</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H16" s="12">
         <v>70</v>
@@ -1720,7 +1731,7 @@
         <v>13</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H17" s="12">
         <v>70</v>
@@ -1748,7 +1759,7 @@
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
       <c r="E18" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G18" s="20"/>
       <c r="H18" s="21">
@@ -1866,25 +1877,25 @@
         <v>11</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="H22" s="21">
         <v>400</v>
       </c>
       <c r="I22" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Customer with contact</v>
+        <v>[GIVEN] Customer with company contact</v>
       </c>
       <c r="J22" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Customer with contact</v>
+        <v>//[GIVEN] Customer with company contact</v>
       </c>
       <c r="K22" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Customer with contact'</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Customer with company contact'</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -1895,25 +1906,25 @@
         <v>11</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="H23" s="21">
         <v>400</v>
       </c>
       <c r="I23" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Closed seminar registration with one participant line</v>
+        <v>[GIVEN] Person contact for customer</v>
       </c>
       <c r="J23" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Closed seminar registration with one participant line</v>
+        <v>//[GIVEN] Person contact for customer</v>
       </c>
       <c r="K23" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Closed seminar registration with one participant line'</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Person contact for customer'</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -1921,25 +1932,25 @@
         <v>26</v>
       </c>
       <c r="F24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="H24" s="21">
         <v>400</v>
       </c>
       <c r="I24" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Post seminar registration</v>
+        <v>[GIVEN] Closed seminar registration with one participant line</v>
       </c>
       <c r="J24" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Post seminar registration</v>
+        <v>//[GIVEN] Closed seminar registration with one participant line</v>
       </c>
       <c r="K24" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Post seminar registration'</v>
+        <v>Given 'Closed seminar registration with one participant line'</v>
       </c>
     </row>
     <row r="25" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -1950,60 +1961,57 @@
         <v>26</v>
       </c>
       <c r="F25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H25" s="21">
         <v>400</v>
       </c>
       <c r="I25" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Seminar registration is removed</v>
+        <v>[WHEN] Post seminar registration</v>
       </c>
       <c r="J25" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Seminar registration is removed</v>
+        <v>//[WHEN] Post seminar registration</v>
       </c>
       <c r="K25" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Seminar registration is removed'</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" s="11" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>When 'Post seminar registration'</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
       <c r="B26" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26"/>
       <c r="F26" t="s">
         <v>13</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H26" s="21">
         <v>400</v>
       </c>
       <c r="I26" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Posted seminar registration exists</v>
+        <v>[THEN] Seminar registration is removed</v>
       </c>
       <c r="J26" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Posted seminar registration exists</v>
+        <v>//[THEN] Seminar registration is removed</v>
       </c>
       <c r="K26" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Posted seminar registration exists'</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" s="11" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Then 'Seminar registration is removed'</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" s="11" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -2017,31 +2025,34 @@
         <v>13</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="H27" s="21">
         <v>400</v>
       </c>
       <c r="I27" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Customer related seminar ledger entry exists</v>
+        <v>[THEN] Posted seminar registration exists</v>
       </c>
       <c r="J27" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Customer related seminar ledger entry exists</v>
+        <v>//[THEN] Posted seminar registration exists</v>
       </c>
       <c r="K27" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Customer related seminar ledger entry exists'</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Then 'Posted seminar registration exists'</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" s="11" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>16</v>
       </c>
       <c r="B28" t="s">
         <v>26</v>
       </c>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28"/>
       <c r="F28" t="s">
         <v>13</v>
       </c>
@@ -2053,18 +2064,18 @@
       </c>
       <c r="I28" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Instructor related seminar ledger entry exists</v>
+        <v>[THEN] Customer related seminar ledger entry exists</v>
       </c>
       <c r="J28" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Instructor related seminar ledger entry exists</v>
+        <v>//[THEN] Customer related seminar ledger entry exists</v>
       </c>
       <c r="K28" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Instructor related seminar ledger entry exists'</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Then 'Customer related seminar ledger entry exists'</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -2082,18 +2093,18 @@
       </c>
       <c r="I29" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Room related seminar ledger entry exists</v>
+        <v>[THEN] Instructor related seminar ledger entry exists</v>
       </c>
       <c r="J29" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Room related seminar ledger entry exists</v>
+        <v>//[THEN] Instructor related seminar ledger entry exists</v>
       </c>
       <c r="K29" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Room related seminar ledger entry exists'</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Then 'Instructor related seminar ledger entry exists'</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -2104,25 +2115,25 @@
         <v>13</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H30" s="21">
         <v>400</v>
       </c>
       <c r="I30" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Instructor related resource ledger entry exists</v>
+        <v>[THEN] Room related seminar ledger entry exists</v>
       </c>
       <c r="J30" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Instructor related resource ledger entry exists</v>
+        <v>//[THEN] Room related seminar ledger entry exists</v>
       </c>
       <c r="K30" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Instructor related resource ledger entry exists'</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Then 'Room related seminar ledger entry exists'</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -2133,88 +2144,85 @@
         <v>13</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H31" s="21">
         <v>400</v>
       </c>
       <c r="I31" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Instructor related resource ledger entry exists</v>
+      </c>
+      <c r="J31" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Instructor related resource ledger entry exists</v>
+      </c>
+      <c r="K31" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Instructor related resource ledger entry exists'</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="H32" s="21">
+        <v>400</v>
+      </c>
+      <c r="I32" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[THEN] Room related resource ledger entry exists</v>
       </c>
-      <c r="J31" s="13" t="str">
+      <c r="J32" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
         <v>//[THEN] Room related resource ledger entry exists</v>
       </c>
-      <c r="K31" s="14" t="str">
+      <c r="K32" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Then 'Room related resource ledger entry exists' }</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B32" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E32" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="F32" s="18"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="21">
+    <row r="33" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="F33" s="18"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="21">
         <v>401</v>
       </c>
-      <c r="I32" s="20" t="str">
+      <c r="I33" s="20" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[SCENARIO #0401] Post non-closed seminar registration</v>
       </c>
-      <c r="J32" s="22" t="str">
+      <c r="J33" s="22" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
         <v>//[SCENARIO #0401] Post non-closed seminar registration</v>
       </c>
-      <c r="K32" s="23" t="str">
+      <c r="K33" s="23" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Scenario 0401 'Post non-closed seminar registration' {</v>
       </c>
-      <c r="L32" s="20"/>
-    </row>
-    <row r="33" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>16</v>
-      </c>
-      <c r="B33" t="s">
-        <v>26</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H33" s="12">
-        <v>401</v>
-      </c>
-      <c r="I33" s="11" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Seminar</v>
-      </c>
-      <c r="J33" s="13" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Seminar</v>
-      </c>
-      <c r="K33" s="14" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Seminar'</v>
-      </c>
+      <c r="L33" s="20"/>
     </row>
     <row r="34" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -2230,22 +2238,22 @@
         <v>11</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="H34" s="12">
         <v>401</v>
       </c>
       <c r="I34" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Instructor resource</v>
+        <v>[GIVEN] Seminar</v>
       </c>
       <c r="J34" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Instructor resource</v>
+        <v>//[GIVEN] Seminar</v>
       </c>
       <c r="K34" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Instructor resource'</v>
+        <v>Given 'Seminar'</v>
       </c>
     </row>
     <row r="35" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2262,22 +2270,22 @@
         <v>11</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H35" s="12">
         <v>401</v>
       </c>
       <c r="I35" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Room resource</v>
+        <v>[GIVEN] Instructor resource</v>
       </c>
       <c r="J35" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Room resource</v>
+        <v>//[GIVEN] Instructor resource</v>
       </c>
       <c r="K35" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Room resource'</v>
+        <v>Given 'Instructor resource'</v>
       </c>
     </row>
     <row r="36" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2294,25 +2302,25 @@
         <v>11</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H36" s="12">
         <v>401</v>
       </c>
       <c r="I36" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Customer with contact</v>
+        <v>[GIVEN] Room resource</v>
       </c>
       <c r="J36" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Customer with contact</v>
+        <v>//[GIVEN] Room resource</v>
       </c>
       <c r="K36" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Customer with contact'</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Room resource'</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>16</v>
       </c>
@@ -2326,22 +2334,22 @@
         <v>11</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="H37" s="12">
         <v>401</v>
       </c>
       <c r="I37" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Non-closed seminar registration with one participant line</v>
+        <v>[GIVEN] Customer with company contact</v>
       </c>
       <c r="J37" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Non-closed seminar registration with one participant line</v>
+        <v>//[GIVEN] Customer with company contact</v>
       </c>
       <c r="K37" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Non-closed seminar registration with one participant line'</v>
+        <v>Given 'Customer with company contact'</v>
       </c>
     </row>
     <row r="38" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2351,29 +2359,26 @@
       <c r="B38" t="s">
         <v>26</v>
       </c>
-      <c r="D38" s="10" t="s">
-        <v>14</v>
-      </c>
       <c r="F38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G38" s="11" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="H38" s="12">
         <v>401</v>
       </c>
       <c r="I38" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Post seminar registration</v>
+        <v>[GIVEN] Person contact for customer</v>
       </c>
       <c r="J38" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Post seminar registration</v>
+        <v>//[GIVEN] Person contact for customer</v>
       </c>
       <c r="K38" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Post seminar registration'</v>
+        <v>Given 'Person contact for customer'</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2387,123 +2392,123 @@
         <v>14</v>
       </c>
       <c r="F39" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="H39" s="12">
         <v>401</v>
       </c>
       <c r="I39" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Non-closed seminar registration with one participant line</v>
+      </c>
+      <c r="J39" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Non-closed seminar registration with one participant line</v>
+      </c>
+      <c r="K39" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Non-closed seminar registration with one participant line'</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F40" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H40" s="12">
+        <v>401</v>
+      </c>
+      <c r="I40" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Post seminar registration</v>
+      </c>
+      <c r="J40" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Post seminar registration</v>
+      </c>
+      <c r="K40" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Post seminar registration'</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="H41" s="12">
+        <v>401</v>
+      </c>
+      <c r="I41" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[THEN] Status must be equal to closed error thrown</v>
       </c>
-      <c r="J39" s="13" t="str">
+      <c r="J41" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
         <v>//[THEN] Status must be equal to closed error thrown</v>
       </c>
-      <c r="K39" s="14" t="str">
+      <c r="K41" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Then 'Status must be equal to closed error thrown' }</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B40" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E40" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="F40" s="18"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="21">
-        <v>402</v>
-      </c>
-      <c r="I40" s="20" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0402] Post closed seminar registration with empty posting date</v>
-      </c>
-      <c r="J40" s="22" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0402] Post closed seminar registration with empty posting date</v>
-      </c>
-      <c r="K40" s="23" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0402 'Post closed seminar registration with empty posting date' {</v>
-      </c>
-      <c r="L40" s="20"/>
-    </row>
-    <row r="41" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>16</v>
-      </c>
-      <c r="B41" t="s">
-        <v>26</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F41" t="s">
-        <v>11</v>
-      </c>
-      <c r="G41" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H41" s="21">
-        <v>402</v>
-      </c>
-      <c r="I41" s="11" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Seminar</v>
-      </c>
-      <c r="J41" s="13" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Seminar</v>
-      </c>
-      <c r="K41" s="14" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Seminar'</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>16</v>
-      </c>
-      <c r="B42" t="s">
-        <v>26</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F42" t="s">
-        <v>11</v>
-      </c>
-      <c r="G42" s="11" t="s">
-        <v>81</v>
-      </c>
+    <row r="42" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="F42" s="18"/>
+      <c r="G42" s="20"/>
       <c r="H42" s="21">
         <v>402</v>
       </c>
-      <c r="I42" s="11" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Instructor resource</v>
-      </c>
-      <c r="J42" s="13" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Instructor resource</v>
-      </c>
-      <c r="K42" s="14" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Instructor resource'</v>
-      </c>
+      <c r="I42" s="20" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0402] Post closed seminar registration with empty posting date</v>
+      </c>
+      <c r="J42" s="22" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0402] Post closed seminar registration with empty posting date</v>
+      </c>
+      <c r="K42" s="23" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0402 'Post closed seminar registration with empty posting date' {</v>
+      </c>
+      <c r="L42" s="20"/>
     </row>
     <row r="43" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -2519,22 +2524,22 @@
         <v>11</v>
       </c>
       <c r="G43" s="11" t="s">
-        <v>82</v>
+        <v>30</v>
       </c>
       <c r="H43" s="21">
         <v>402</v>
       </c>
       <c r="I43" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Room resource</v>
+        <v>[GIVEN] Seminar</v>
       </c>
       <c r="J43" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Room resource</v>
+        <v>//[GIVEN] Seminar</v>
       </c>
       <c r="K43" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Room resource'</v>
+        <v>Given 'Seminar'</v>
       </c>
     </row>
     <row r="44" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2551,25 +2556,25 @@
         <v>11</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="H44" s="21">
         <v>402</v>
       </c>
       <c r="I44" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Customer with contact</v>
+        <v>[GIVEN] Instructor resource</v>
       </c>
       <c r="J44" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Customer with contact</v>
+        <v>//[GIVEN] Instructor resource</v>
       </c>
       <c r="K44" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Customer with contact'</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Instructor resource'</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>16</v>
       </c>
@@ -2583,22 +2588,22 @@
         <v>11</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="H45" s="21">
         <v>402</v>
       </c>
       <c r="I45" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Closed seminar registration with one participant line and empty posting date</v>
+        <v>[GIVEN] Room resource</v>
       </c>
       <c r="J45" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Closed seminar registration with one participant line and empty posting date</v>
+        <v>//[GIVEN] Room resource</v>
       </c>
       <c r="K45" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Closed seminar registration with one participant line and empty posting date'</v>
+        <v>Given 'Room resource'</v>
       </c>
     </row>
     <row r="46" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2612,91 +2617,87 @@
         <v>14</v>
       </c>
       <c r="F46" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="H46" s="21">
         <v>402</v>
       </c>
       <c r="I46" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Post seminar registration</v>
+        <v>[GIVEN] Customer with company contact</v>
       </c>
       <c r="J46" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Post seminar registration</v>
+        <v>//[GIVEN] Customer with company contact</v>
       </c>
       <c r="K46" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Post seminar registration'</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Customer with company contact'</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>16</v>
       </c>
       <c r="B47" t="s">
         <v>26</v>
       </c>
-      <c r="D47" s="10" t="s">
-        <v>14</v>
-      </c>
       <c r="F47" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="H47" s="21">
         <v>402</v>
       </c>
       <c r="I47" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Posting date must be have value error thrown</v>
+        <v>[GIVEN] Person contact for customer</v>
       </c>
       <c r="J47" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Posting date must be have value error thrown</v>
+        <v>//[GIVEN] Person contact for customer</v>
       </c>
       <c r="K47" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Posting date must be have value error thrown' }</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B48" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E48" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="20"/>
+        <v>Given 'Person contact for customer'</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F48" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" s="11" t="s">
+        <v>101</v>
+      </c>
       <c r="H48" s="21">
-        <v>403</v>
-      </c>
-      <c r="I48" s="20" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0403] Post closed seminar registration with empty document date</v>
-      </c>
-      <c r="J48" s="22" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0403] Post closed seminar registration with empty document date</v>
-      </c>
-      <c r="K48" s="23" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0403 'Post closed seminar registration with empty document date' {</v>
-      </c>
-      <c r="L48" s="20"/>
+        <v>402</v>
+      </c>
+      <c r="I48" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Closed seminar registration with one participant line and empty posting date</v>
+      </c>
+      <c r="J48" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Closed seminar registration with one participant line and empty posting date</v>
+      </c>
+      <c r="K48" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Closed seminar registration with one participant line and empty posting date'</v>
+      </c>
     </row>
     <row r="49" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
@@ -2709,90 +2710,91 @@
         <v>14</v>
       </c>
       <c r="F49" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H49" s="12">
+        <v>86</v>
+      </c>
+      <c r="H49" s="21">
+        <v>402</v>
+      </c>
+      <c r="I49" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Post seminar registration</v>
+      </c>
+      <c r="J49" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Post seminar registration</v>
+      </c>
+      <c r="K49" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Post seminar registration'</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F50" t="s">
+        <v>13</v>
+      </c>
+      <c r="G50" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="H50" s="21">
+        <v>402</v>
+      </c>
+      <c r="I50" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Posting date must be have value error thrown</v>
+      </c>
+      <c r="J50" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Posting date must be have value error thrown</v>
+      </c>
+      <c r="K50" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Posting date must be have value error thrown' }</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B51" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E51" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="F51" s="18"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="21">
         <v>403</v>
       </c>
-      <c r="I49" s="11" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Seminar</v>
-      </c>
-      <c r="J49" s="13" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Seminar</v>
-      </c>
-      <c r="K49" s="14" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Seminar'</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>16</v>
-      </c>
-      <c r="B50" t="s">
-        <v>26</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F50" t="s">
-        <v>11</v>
-      </c>
-      <c r="G50" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="H50" s="12">
-        <v>403</v>
-      </c>
-      <c r="I50" s="11" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Instructor resource</v>
-      </c>
-      <c r="J50" s="13" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Instructor resource</v>
-      </c>
-      <c r="K50" s="14" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Instructor resource'</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>16</v>
-      </c>
-      <c r="B51" t="s">
-        <v>26</v>
-      </c>
-      <c r="D51" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F51" t="s">
-        <v>11</v>
-      </c>
-      <c r="G51" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="H51" s="12">
-        <v>403</v>
-      </c>
-      <c r="I51" s="11" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Room resource</v>
-      </c>
-      <c r="J51" s="13" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Room resource</v>
-      </c>
-      <c r="K51" s="14" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Room resource'</v>
-      </c>
+      <c r="I51" s="20" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0403] Post closed seminar registration with empty document date</v>
+      </c>
+      <c r="J51" s="22" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0403] Post closed seminar registration with empty document date</v>
+      </c>
+      <c r="K51" s="23" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0403 'Post closed seminar registration with empty document date' {</v>
+      </c>
+      <c r="L51" s="20"/>
     </row>
     <row r="52" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
@@ -2808,25 +2810,25 @@
         <v>11</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="H52" s="12">
         <v>403</v>
       </c>
       <c r="I52" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Customer with contact</v>
+        <v>[GIVEN] Seminar</v>
       </c>
       <c r="J52" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Customer with contact</v>
+        <v>//[GIVEN] Seminar</v>
       </c>
       <c r="K52" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Customer with contact'</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Seminar'</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>16</v>
       </c>
@@ -2840,22 +2842,22 @@
         <v>11</v>
       </c>
       <c r="G53" s="11" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="H53" s="12">
         <v>403</v>
       </c>
       <c r="I53" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Closed seminar registration with one participant line and empty document date</v>
+        <v>[GIVEN] Instructor resource</v>
       </c>
       <c r="J53" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Closed seminar registration with one participant line and empty document date</v>
+        <v>//[GIVEN] Instructor resource</v>
       </c>
       <c r="K53" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Closed seminar registration with one participant line and empty document date'</v>
+        <v>Given 'Instructor resource'</v>
       </c>
     </row>
     <row r="54" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2869,28 +2871,28 @@
         <v>14</v>
       </c>
       <c r="F54" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G54" s="11" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H54" s="12">
         <v>403</v>
       </c>
       <c r="I54" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Post seminar registration</v>
+        <v>[GIVEN] Room resource</v>
       </c>
       <c r="J54" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Post seminar registration</v>
+        <v>//[GIVEN] Room resource</v>
       </c>
       <c r="K54" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Post seminar registration'</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Room resource'</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>16</v>
       </c>
@@ -2901,61 +2903,57 @@
         <v>14</v>
       </c>
       <c r="F55" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G55" s="11" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="H55" s="12">
         <v>403</v>
       </c>
       <c r="I55" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Document date must be have value error thrown</v>
+        <v>[GIVEN] Customer with company contact</v>
       </c>
       <c r="J55" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Document date must be have value error thrown</v>
+        <v>//[GIVEN] Customer with company contact</v>
       </c>
       <c r="K55" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Document date must be have value error thrown' }</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B56" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C56" s="19"/>
-      <c r="D56" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E56" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="F56" s="18"/>
-      <c r="G56" s="20"/>
-      <c r="H56" s="21">
-        <v>404</v>
-      </c>
-      <c r="I56" s="20" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0404] Post closed seminar registration with empty seminar number</v>
-      </c>
-      <c r="J56" s="22" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0404] Post closed seminar registration with empty seminar number</v>
-      </c>
-      <c r="K56" s="23" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0404 'Post closed seminar registration with empty seminar number' {</v>
-      </c>
-      <c r="L56" s="20"/>
-    </row>
-    <row r="57" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Customer with company contact'</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>16</v>
+      </c>
+      <c r="B56" t="s">
+        <v>26</v>
+      </c>
+      <c r="F56" t="s">
+        <v>11</v>
+      </c>
+      <c r="G56" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="H56" s="12">
+        <v>403</v>
+      </c>
+      <c r="I56" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Person contact for customer</v>
+      </c>
+      <c r="J56" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Person contact for customer</v>
+      </c>
+      <c r="K56" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Person contact for customer'</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>16</v>
       </c>
@@ -2969,22 +2967,22 @@
         <v>11</v>
       </c>
       <c r="G57" s="11" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="H57" s="12">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="I57" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Seminar</v>
+        <v>[GIVEN] Closed seminar registration with one participant line and empty document date</v>
       </c>
       <c r="J57" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Seminar</v>
+        <v>//[GIVEN] Closed seminar registration with one participant line and empty document date</v>
       </c>
       <c r="K57" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Seminar'</v>
+        <v>Given 'Closed seminar registration with one participant line and empty document date'</v>
       </c>
     </row>
     <row r="58" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -2998,92 +2996,93 @@
         <v>14</v>
       </c>
       <c r="F58" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="H58" s="12">
+        <v>403</v>
+      </c>
+      <c r="I58" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Post seminar registration</v>
+      </c>
+      <c r="J58" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Post seminar registration</v>
+      </c>
+      <c r="K58" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Post seminar registration'</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>16</v>
+      </c>
+      <c r="B59" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F59" t="s">
+        <v>13</v>
+      </c>
+      <c r="G59" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="H59" s="12">
+        <v>403</v>
+      </c>
+      <c r="I59" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Document date must be have value error thrown</v>
+      </c>
+      <c r="J59" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Document date must be have value error thrown</v>
+      </c>
+      <c r="K59" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Document date must be have value error thrown' }</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B60" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C60" s="19"/>
+      <c r="D60" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E60" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="F60" s="18"/>
+      <c r="G60" s="20"/>
+      <c r="H60" s="21">
         <v>404</v>
       </c>
-      <c r="I58" s="11" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Instructor resource</v>
-      </c>
-      <c r="J58" s="13" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Instructor resource</v>
-      </c>
-      <c r="K58" s="14" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Instructor resource'</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>16</v>
-      </c>
-      <c r="B59" t="s">
-        <v>26</v>
-      </c>
-      <c r="D59" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F59" t="s">
-        <v>11</v>
-      </c>
-      <c r="G59" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="H59" s="12">
-        <v>404</v>
-      </c>
-      <c r="I59" s="11" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Room resource</v>
-      </c>
-      <c r="J59" s="13" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Room resource</v>
-      </c>
-      <c r="K59" s="14" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Room resource'</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>16</v>
-      </c>
-      <c r="B60" t="s">
-        <v>26</v>
-      </c>
-      <c r="D60" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F60" t="s">
-        <v>11</v>
-      </c>
-      <c r="G60" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="H60" s="12">
-        <v>404</v>
-      </c>
-      <c r="I60" s="11" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Customer with contact</v>
-      </c>
-      <c r="J60" s="13" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Customer with contact</v>
-      </c>
-      <c r="K60" s="14" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Customer with contact'</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="I60" s="20" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0404] Post closed seminar registration with empty seminar number</v>
+      </c>
+      <c r="J60" s="22" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0404] Post closed seminar registration with empty seminar number</v>
+      </c>
+      <c r="K60" s="23" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0404 'Post closed seminar registration with empty seminar number' {</v>
+      </c>
+      <c r="L60" s="20"/>
+    </row>
+    <row r="61" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>16</v>
       </c>
@@ -3097,22 +3096,22 @@
         <v>11</v>
       </c>
       <c r="G61" s="11" t="s">
-        <v>108</v>
+        <v>30</v>
       </c>
       <c r="H61" s="12">
         <v>404</v>
       </c>
       <c r="I61" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Closed seminar registration with one participant line and empty seminar number</v>
+        <v>[GIVEN] Seminar</v>
       </c>
       <c r="J61" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Closed seminar registration with one participant line and empty seminar number</v>
+        <v>//[GIVEN] Seminar</v>
       </c>
       <c r="K61" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Closed seminar registration with one participant line and empty seminar number'</v>
+        <v>Given 'Seminar'</v>
       </c>
     </row>
     <row r="62" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3126,28 +3125,28 @@
         <v>14</v>
       </c>
       <c r="F62" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G62" s="11" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H62" s="12">
         <v>404</v>
       </c>
       <c r="I62" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Post seminar registration</v>
+        <v>[GIVEN] Instructor resource</v>
       </c>
       <c r="J62" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Post seminar registration</v>
+        <v>//[GIVEN] Instructor resource</v>
       </c>
       <c r="K62" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Post seminar registration'</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Instructor resource'</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>16</v>
       </c>
@@ -3158,59 +3157,58 @@
         <v>14</v>
       </c>
       <c r="F63" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>109</v>
+        <v>82</v>
       </c>
       <c r="H63" s="12">
         <v>404</v>
       </c>
       <c r="I63" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Seminar number must be have value error thrown</v>
+        <v>[GIVEN] Room resource</v>
       </c>
       <c r="J63" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Seminar number must be have value error thrown</v>
+        <v>//[GIVEN] Room resource</v>
       </c>
       <c r="K63" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Seminar number must be have value error thrown' }</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B64" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C64" s="19"/>
-      <c r="D64" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E64" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="F64" s="18"/>
-      <c r="G64" s="20"/>
-      <c r="H64" s="21">
-        <v>405</v>
-      </c>
-      <c r="I64" s="20" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0405] Post closed seminar registration with empty duration</v>
-      </c>
-      <c r="J64" s="22" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0405] Post closed seminar registration with empty duration</v>
-      </c>
-      <c r="K64" s="23" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0405 'Post closed seminar registration with empty duration' {</v>
-      </c>
-      <c r="L64" s="20"/>
+        <v>Given 'Room resource'</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>16</v>
+      </c>
+      <c r="B64" t="s">
+        <v>26</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F64" t="s">
+        <v>11</v>
+      </c>
+      <c r="G64" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="H64" s="12">
+        <v>404</v>
+      </c>
+      <c r="I64" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Customer with company contact</v>
+      </c>
+      <c r="J64" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Customer with company contact</v>
+      </c>
+      <c r="K64" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Customer with company contact'</v>
+      </c>
     </row>
     <row r="65" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
@@ -3219,32 +3217,29 @@
       <c r="B65" t="s">
         <v>26</v>
       </c>
-      <c r="D65" s="10" t="s">
-        <v>14</v>
-      </c>
       <c r="F65" t="s">
         <v>11</v>
       </c>
       <c r="G65" s="11" t="s">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="H65" s="12">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="I65" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Seminar</v>
+        <v>[GIVEN] Person contact for customer</v>
       </c>
       <c r="J65" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Seminar</v>
+        <v>//[GIVEN] Person contact for customer</v>
       </c>
       <c r="K65" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Seminar'</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Person contact for customer'</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>16</v>
       </c>
@@ -3258,22 +3253,22 @@
         <v>11</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="H66" s="12">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="I66" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Instructor resource</v>
+        <v>[GIVEN] Closed seminar registration with one participant line and empty seminar number</v>
       </c>
       <c r="J66" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Instructor resource</v>
+        <v>//[GIVEN] Closed seminar registration with one participant line and empty seminar number</v>
       </c>
       <c r="K66" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Instructor resource'</v>
+        <v>Given 'Closed seminar registration with one participant line and empty seminar number'</v>
       </c>
     </row>
     <row r="67" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3287,90 +3282,91 @@
         <v>14</v>
       </c>
       <c r="F67" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G67" s="11" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="H67" s="12">
+        <v>404</v>
+      </c>
+      <c r="I67" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Post seminar registration</v>
+      </c>
+      <c r="J67" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Post seminar registration</v>
+      </c>
+      <c r="K67" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Post seminar registration'</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>16</v>
+      </c>
+      <c r="B68" t="s">
+        <v>26</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F68" t="s">
+        <v>13</v>
+      </c>
+      <c r="G68" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="H68" s="12">
+        <v>404</v>
+      </c>
+      <c r="I68" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Seminar number must be have value error thrown</v>
+      </c>
+      <c r="J68" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Seminar number must be have value error thrown</v>
+      </c>
+      <c r="K68" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Seminar number must be have value error thrown' }</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B69" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C69" s="19"/>
+      <c r="D69" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E69" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="F69" s="18"/>
+      <c r="G69" s="20"/>
+      <c r="H69" s="21">
         <v>405</v>
       </c>
-      <c r="I67" s="11" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Room resource</v>
-      </c>
-      <c r="J67" s="13" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Room resource</v>
-      </c>
-      <c r="K67" s="14" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Room resource'</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>16</v>
-      </c>
-      <c r="B68" t="s">
-        <v>26</v>
-      </c>
-      <c r="D68" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F68" t="s">
-        <v>11</v>
-      </c>
-      <c r="G68" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="H68" s="12">
-        <v>405</v>
-      </c>
-      <c r="I68" s="11" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Customer with contact</v>
-      </c>
-      <c r="J68" s="13" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Customer with contact</v>
-      </c>
-      <c r="K68" s="14" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Customer with contact'</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>16</v>
-      </c>
-      <c r="B69" t="s">
-        <v>26</v>
-      </c>
-      <c r="D69" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F69" t="s">
-        <v>11</v>
-      </c>
-      <c r="G69" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="H69" s="12">
-        <v>405</v>
-      </c>
-      <c r="I69" s="11" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Closed seminar registration with one participant line and empty duration</v>
-      </c>
-      <c r="J69" s="13" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Closed seminar registration with one participant line and empty duration</v>
-      </c>
-      <c r="K69" s="14" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Closed seminar registration with one participant line and empty duration'</v>
-      </c>
+      <c r="I69" s="20" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0405] Post closed seminar registration with empty duration</v>
+      </c>
+      <c r="J69" s="22" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0405] Post closed seminar registration with empty duration</v>
+      </c>
+      <c r="K69" s="23" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0405 'Post closed seminar registration with empty duration' {</v>
+      </c>
+      <c r="L69" s="20"/>
     </row>
     <row r="70" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
@@ -3383,28 +3379,28 @@
         <v>14</v>
       </c>
       <c r="F70" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G70" s="11" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="H70" s="12">
         <v>405</v>
       </c>
       <c r="I70" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Post seminar registration</v>
+        <v>[GIVEN] Seminar</v>
       </c>
       <c r="J70" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Post seminar registration</v>
+        <v>//[GIVEN] Seminar</v>
       </c>
       <c r="K70" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Post seminar registration'</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Seminar'</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>16</v>
       </c>
@@ -3415,59 +3411,58 @@
         <v>14</v>
       </c>
       <c r="F71" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G71" s="11" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="H71" s="12">
         <v>405</v>
       </c>
       <c r="I71" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Duration must be have value error thrown</v>
+        <v>[GIVEN] Instructor resource</v>
       </c>
       <c r="J71" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Duration must be have value error thrown</v>
+        <v>//[GIVEN] Instructor resource</v>
       </c>
       <c r="K71" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Duration must be have value error thrown' }</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" ht="28.5" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B72" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C72" s="19"/>
-      <c r="D72" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E72" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="F72" s="18"/>
-      <c r="G72" s="20"/>
-      <c r="H72" s="21">
-        <v>406</v>
-      </c>
-      <c r="I72" s="20" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0406] Post closed seminar registration with empty instructor resource number</v>
-      </c>
-      <c r="J72" s="22" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0406] Post closed seminar registration with empty instructor resource number</v>
-      </c>
-      <c r="K72" s="23" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0406 'Post closed seminar registration with empty instructor resource number' {</v>
-      </c>
-      <c r="L72" s="20"/>
+        <v>Given 'Instructor resource'</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>16</v>
+      </c>
+      <c r="B72" t="s">
+        <v>26</v>
+      </c>
+      <c r="D72" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F72" t="s">
+        <v>11</v>
+      </c>
+      <c r="G72" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H72" s="12">
+        <v>405</v>
+      </c>
+      <c r="I72" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Room resource</v>
+      </c>
+      <c r="J72" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Room resource</v>
+      </c>
+      <c r="K72" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Room resource'</v>
+      </c>
     </row>
     <row r="73" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
@@ -3483,22 +3478,22 @@
         <v>11</v>
       </c>
       <c r="G73" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H73" s="21">
-        <v>406</v>
+        <v>92</v>
+      </c>
+      <c r="H73" s="12">
+        <v>405</v>
       </c>
       <c r="I73" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Seminar</v>
+        <v>[GIVEN] Customer with company contact</v>
       </c>
       <c r="J73" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Seminar</v>
+        <v>//[GIVEN] Customer with company contact</v>
       </c>
       <c r="K73" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Seminar'</v>
+        <v>Given 'Customer with company contact'</v>
       </c>
     </row>
     <row r="74" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3508,32 +3503,29 @@
       <c r="B74" t="s">
         <v>26</v>
       </c>
-      <c r="D74" s="10" t="s">
-        <v>14</v>
-      </c>
       <c r="F74" t="s">
         <v>11</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="H74" s="21">
-        <v>406</v>
+        <v>93</v>
+      </c>
+      <c r="H74" s="12">
+        <v>405</v>
       </c>
       <c r="I74" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Instructor resource</v>
+        <v>[GIVEN] Person contact for customer</v>
       </c>
       <c r="J74" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Instructor resource</v>
+        <v>//[GIVEN] Person contact for customer</v>
       </c>
       <c r="K74" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Instructor resource'</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Person contact for customer'</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>16</v>
       </c>
@@ -3547,22 +3539,22 @@
         <v>11</v>
       </c>
       <c r="G75" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="H75" s="21">
-        <v>406</v>
+        <v>110</v>
+      </c>
+      <c r="H75" s="12">
+        <v>405</v>
       </c>
       <c r="I75" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Room resource</v>
+        <v>[GIVEN] Closed seminar registration with one participant line and empty duration</v>
       </c>
       <c r="J75" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Room resource</v>
+        <v>//[GIVEN] Closed seminar registration with one participant line and empty duration</v>
       </c>
       <c r="K75" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Room resource'</v>
+        <v>Given 'Closed seminar registration with one participant line and empty duration'</v>
       </c>
     </row>
     <row r="76" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3576,28 +3568,28 @@
         <v>14</v>
       </c>
       <c r="F76" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G76" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="H76" s="21">
-        <v>406</v>
+        <v>86</v>
+      </c>
+      <c r="H76" s="12">
+        <v>405</v>
       </c>
       <c r="I76" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Customer with contact</v>
+        <v>[WHEN] Post seminar registration</v>
       </c>
       <c r="J76" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Customer with contact</v>
+        <v>//[WHEN] Post seminar registration</v>
       </c>
       <c r="K76" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Customer with contact'</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>When 'Post seminar registration'</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>16</v>
       </c>
@@ -3608,60 +3600,61 @@
         <v>14</v>
       </c>
       <c r="F77" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G77" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="H77" s="21">
-        <v>406</v>
+        <v>111</v>
+      </c>
+      <c r="H77" s="12">
+        <v>405</v>
       </c>
       <c r="I77" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Closed seminar registration with one participant line and empty instructor resource number</v>
+        <v>[THEN] Duration must be have value error thrown</v>
       </c>
       <c r="J77" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Closed seminar registration with one participant line and empty instructor resource number</v>
+        <v>//[THEN] Duration must be have value error thrown</v>
       </c>
       <c r="K77" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Closed seminar registration with one participant line and empty instructor resource number'</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>16</v>
-      </c>
-      <c r="B78" t="s">
-        <v>26</v>
-      </c>
-      <c r="D78" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F78" t="s">
-        <v>12</v>
-      </c>
-      <c r="G78" s="11" t="s">
-        <v>86</v>
-      </c>
+        <v>Then 'Duration must be have value error thrown' }</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="28.5" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B78" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C78" s="19"/>
+      <c r="D78" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E78" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="F78" s="18"/>
+      <c r="G78" s="20"/>
       <c r="H78" s="21">
         <v>406</v>
       </c>
-      <c r="I78" s="11" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Post seminar registration</v>
-      </c>
-      <c r="J78" s="13" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Post seminar registration</v>
-      </c>
-      <c r="K78" s="14" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Post seminar registration'</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="I78" s="20" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0406] Post closed seminar registration with empty instructor resource number</v>
+      </c>
+      <c r="J78" s="22" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0406] Post closed seminar registration with empty instructor resource number</v>
+      </c>
+      <c r="K78" s="23" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0406 'Post closed seminar registration with empty instructor resource number' {</v>
+      </c>
+      <c r="L78" s="20"/>
+    </row>
+    <row r="79" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>16</v>
       </c>
@@ -3672,59 +3665,58 @@
         <v>14</v>
       </c>
       <c r="F79" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G79" s="11" t="s">
-        <v>115</v>
+        <v>30</v>
       </c>
       <c r="H79" s="21">
         <v>406</v>
       </c>
       <c r="I79" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Instructor resource number must be have value error thrown</v>
+        <v>[GIVEN] Seminar</v>
       </c>
       <c r="J79" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Instructor resource number must be have value error thrown</v>
+        <v>//[GIVEN] Seminar</v>
       </c>
       <c r="K79" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Instructor resource number must be have value error thrown' }</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" ht="33" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B80" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C80" s="19"/>
-      <c r="D80" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E80" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="F80" s="18"/>
-      <c r="G80" s="20"/>
+        <v>Given 'Seminar'</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>16</v>
+      </c>
+      <c r="B80" t="s">
+        <v>26</v>
+      </c>
+      <c r="D80" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F80" t="s">
+        <v>11</v>
+      </c>
+      <c r="G80" s="11" t="s">
+        <v>81</v>
+      </c>
       <c r="H80" s="21">
-        <v>407</v>
-      </c>
-      <c r="I80" s="20" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0407] Post closed seminar registration with empty room resource number</v>
-      </c>
-      <c r="J80" s="22" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0407] Post closed seminar registration with empty room resource number</v>
-      </c>
-      <c r="K80" s="23" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0407 'Post closed seminar registration with empty room resource number' {</v>
-      </c>
-      <c r="L80" s="20"/>
+        <v>406</v>
+      </c>
+      <c r="I80" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Instructor resource</v>
+      </c>
+      <c r="J80" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Instructor resource</v>
+      </c>
+      <c r="K80" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Instructor resource'</v>
+      </c>
     </row>
     <row r="81" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
@@ -3740,22 +3732,22 @@
         <v>11</v>
       </c>
       <c r="G81" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H81" s="12">
-        <v>407</v>
+        <v>82</v>
+      </c>
+      <c r="H81" s="21">
+        <v>406</v>
       </c>
       <c r="I81" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Seminar</v>
+        <v>[GIVEN] Room resource</v>
       </c>
       <c r="J81" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Seminar</v>
+        <v>//[GIVEN] Room resource</v>
       </c>
       <c r="K81" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Seminar'</v>
+        <v>Given 'Room resource'</v>
       </c>
     </row>
     <row r="82" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3772,22 +3764,22 @@
         <v>11</v>
       </c>
       <c r="G82" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="H82" s="12">
-        <v>407</v>
+        <v>92</v>
+      </c>
+      <c r="H82" s="21">
+        <v>406</v>
       </c>
       <c r="I82" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Instructor resource</v>
+        <v>[GIVEN] Customer with company contact</v>
       </c>
       <c r="J82" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Instructor resource</v>
+        <v>//[GIVEN] Customer with company contact</v>
       </c>
       <c r="K82" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Instructor resource'</v>
+        <v>Given 'Customer with company contact'</v>
       </c>
     </row>
     <row r="83" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -3797,191 +3789,188 @@
       <c r="B83" t="s">
         <v>26</v>
       </c>
-      <c r="D83" s="10" t="s">
-        <v>14</v>
-      </c>
       <c r="F83" t="s">
         <v>11</v>
       </c>
       <c r="G83" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="H83" s="12">
+        <v>93</v>
+      </c>
+      <c r="H83" s="21">
+        <v>406</v>
+      </c>
+      <c r="I83" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Person contact for customer</v>
+      </c>
+      <c r="J83" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Person contact for customer</v>
+      </c>
+      <c r="K83" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Person contact for customer'</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>16</v>
+      </c>
+      <c r="B84" t="s">
+        <v>26</v>
+      </c>
+      <c r="D84" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F84" t="s">
+        <v>11</v>
+      </c>
+      <c r="G84" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="H84" s="21">
+        <v>406</v>
+      </c>
+      <c r="I84" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Closed seminar registration with one participant line and empty instructor resource number</v>
+      </c>
+      <c r="J84" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Closed seminar registration with one participant line and empty instructor resource number</v>
+      </c>
+      <c r="K84" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Closed seminar registration with one participant line and empty instructor resource number'</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>16</v>
+      </c>
+      <c r="B85" t="s">
+        <v>26</v>
+      </c>
+      <c r="D85" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F85" t="s">
+        <v>12</v>
+      </c>
+      <c r="G85" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H85" s="21">
+        <v>406</v>
+      </c>
+      <c r="I85" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Post seminar registration</v>
+      </c>
+      <c r="J85" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Post seminar registration</v>
+      </c>
+      <c r="K85" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Post seminar registration'</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>16</v>
+      </c>
+      <c r="B86" t="s">
+        <v>26</v>
+      </c>
+      <c r="D86" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F86" t="s">
+        <v>13</v>
+      </c>
+      <c r="G86" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="H86" s="21">
+        <v>406</v>
+      </c>
+      <c r="I86" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Instructor resource number must be have value error thrown</v>
+      </c>
+      <c r="J86" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Instructor resource number must be have value error thrown</v>
+      </c>
+      <c r="K86" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Instructor resource number must be have value error thrown' }</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" ht="33" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B87" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C87" s="19"/>
+      <c r="D87" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E87" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="F87" s="18"/>
+      <c r="G87" s="20"/>
+      <c r="H87" s="21">
         <v>407</v>
       </c>
-      <c r="I83" s="11" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Room resource</v>
-      </c>
-      <c r="J83" s="13" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Room resource</v>
-      </c>
-      <c r="K83" s="14" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Room resource'</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>16</v>
-      </c>
-      <c r="B84" t="s">
-        <v>26</v>
-      </c>
-      <c r="D84" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F84" t="s">
-        <v>11</v>
-      </c>
-      <c r="G84" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="H84" s="12">
+      <c r="I87" s="20" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0407] Post closed seminar registration with empty room resource number</v>
+      </c>
+      <c r="J87" s="22" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0407] Post closed seminar registration with empty room resource number</v>
+      </c>
+      <c r="K87" s="23" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0407 'Post closed seminar registration with empty room resource number' {</v>
+      </c>
+      <c r="L87" s="20"/>
+    </row>
+    <row r="88" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>16</v>
+      </c>
+      <c r="B88" t="s">
+        <v>26</v>
+      </c>
+      <c r="D88" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F88" t="s">
+        <v>11</v>
+      </c>
+      <c r="G88" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H88" s="12">
         <v>407</v>
       </c>
-      <c r="I84" s="11" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Customer with contact</v>
-      </c>
-      <c r="J84" s="13" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Customer with contact</v>
-      </c>
-      <c r="K84" s="14" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Customer with contact'</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>16</v>
-      </c>
-      <c r="B85" t="s">
-        <v>26</v>
-      </c>
-      <c r="D85" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F85" t="s">
-        <v>11</v>
-      </c>
-      <c r="G85" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="H85" s="12">
-        <v>407</v>
-      </c>
-      <c r="I85" s="11" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Closed seminar registration with one participant line and empty room resource number</v>
-      </c>
-      <c r="J85" s="13" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Closed seminar registration with one participant line and empty room resource number</v>
-      </c>
-      <c r="K85" s="14" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Closed seminar registration with one participant line and empty room resource number'</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>16</v>
-      </c>
-      <c r="B86" t="s">
-        <v>26</v>
-      </c>
-      <c r="D86" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F86" t="s">
-        <v>12</v>
-      </c>
-      <c r="G86" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="H86" s="12">
-        <v>407</v>
-      </c>
-      <c r="I86" s="11" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Post seminar registration</v>
-      </c>
-      <c r="J86" s="13" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Post seminar registration</v>
-      </c>
-      <c r="K86" s="14" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Post seminar registration'</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>16</v>
-      </c>
-      <c r="B87" t="s">
-        <v>26</v>
-      </c>
-      <c r="D87" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F87" t="s">
-        <v>13</v>
-      </c>
-      <c r="G87" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="H87" s="12">
-        <v>407</v>
-      </c>
-      <c r="I87" s="11" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[THEN] Room resource number must be have value error thrown</v>
-      </c>
-      <c r="J87" s="13" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[THEN] Room resource number must be have value error thrown</v>
-      </c>
-      <c r="K87" s="14" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Then 'Room resource number must be have value error thrown' }</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B88" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C88" s="19"/>
-      <c r="D88" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E88" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="F88" s="18"/>
-      <c r="G88" s="20"/>
-      <c r="H88" s="21">
-        <v>408</v>
-      </c>
-      <c r="I88" s="20" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0408] Post closed seminar registration with no participant line</v>
-      </c>
-      <c r="J88" s="22" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0408] Post closed seminar registration with no participant line</v>
-      </c>
-      <c r="K88" s="23" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0408 'Post closed seminar registration with no participant line' {</v>
-      </c>
-      <c r="L88" s="20"/>
+      <c r="I88" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Seminar</v>
+      </c>
+      <c r="J88" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Seminar</v>
+      </c>
+      <c r="K88" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Seminar'</v>
+      </c>
     </row>
     <row r="89" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
@@ -3997,22 +3986,22 @@
         <v>11</v>
       </c>
       <c r="G89" s="11" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="H89" s="12">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="I89" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Seminar</v>
+        <v>[GIVEN] Instructor resource</v>
       </c>
       <c r="J89" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Seminar</v>
+        <v>//[GIVEN] Instructor resource</v>
       </c>
       <c r="K89" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Seminar'</v>
+        <v>Given 'Instructor resource'</v>
       </c>
     </row>
     <row r="90" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4029,22 +4018,22 @@
         <v>11</v>
       </c>
       <c r="G90" s="11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H90" s="12">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="I90" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Instructor resource</v>
+        <v>[GIVEN] Room resource</v>
       </c>
       <c r="J90" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Instructor resource</v>
+        <v>//[GIVEN] Room resource</v>
       </c>
       <c r="K90" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Instructor resource'</v>
+        <v>Given 'Room resource'</v>
       </c>
     </row>
     <row r="91" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4061,57 +4050,54 @@
         <v>11</v>
       </c>
       <c r="G91" s="11" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="H91" s="12">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="I91" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Room resource</v>
+        <v>[GIVEN] Customer with company contact</v>
       </c>
       <c r="J91" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Room resource</v>
+        <v>//[GIVEN] Customer with company contact</v>
       </c>
       <c r="K91" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Room resource'</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Customer with company contact'</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>16</v>
       </c>
       <c r="B92" t="s">
         <v>26</v>
       </c>
-      <c r="D92" s="10" t="s">
-        <v>14</v>
-      </c>
       <c r="F92" t="s">
         <v>11</v>
       </c>
       <c r="G92" s="11" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="H92" s="12">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="I92" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[GIVEN] Closed seminar registration with no participant line</v>
+        <v>[GIVEN] Person contact for customer</v>
       </c>
       <c r="J92" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[GIVEN] Closed seminar registration with no participant line</v>
+        <v>//[GIVEN] Person contact for customer</v>
       </c>
       <c r="K92" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Given 'Closed seminar registration with no participant line'</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>Given 'Person contact for customer'</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>16</v>
       </c>
@@ -4122,25 +4108,25 @@
         <v>14</v>
       </c>
       <c r="F93" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G93" s="11" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="H93" s="12">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="I93" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[WHEN] Post seminar registration</v>
+        <v>[GIVEN] Closed seminar registration with one participant line and empty room resource number</v>
       </c>
       <c r="J93" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[WHEN] Post seminar registration</v>
+        <v>//[GIVEN] Closed seminar registration with one participant line and empty room resource number</v>
       </c>
       <c r="K93" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>When 'Post seminar registration'</v>
+        <v>Given 'Closed seminar registration with one participant line and empty room resource number'</v>
       </c>
     </row>
     <row r="94" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -4154,61 +4140,774 @@
         <v>14</v>
       </c>
       <c r="F94" t="s">
+        <v>12</v>
+      </c>
+      <c r="G94" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H94" s="12">
+        <v>407</v>
+      </c>
+      <c r="I94" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Post seminar registration</v>
+      </c>
+      <c r="J94" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Post seminar registration</v>
+      </c>
+      <c r="K94" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Post seminar registration'</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>16</v>
+      </c>
+      <c r="B95" t="s">
+        <v>26</v>
+      </c>
+      <c r="D95" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F95" t="s">
         <v>13</v>
       </c>
-      <c r="G94" s="11" t="s">
+      <c r="G95" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="H95" s="12">
+        <v>407</v>
+      </c>
+      <c r="I95" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Room resource number must be have value error thrown</v>
+      </c>
+      <c r="J95" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Room resource number must be have value error thrown</v>
+      </c>
+      <c r="K95" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Room resource number must be have value error thrown' }</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" ht="30" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B96" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C96" s="19"/>
+      <c r="D96" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E96" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="H94" s="12">
+      <c r="F96" s="18"/>
+      <c r="G96" s="20"/>
+      <c r="H96" s="21">
         <v>408</v>
       </c>
-      <c r="I94" s="11" t="str">
+      <c r="I96" s="20" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0408] Post closed seminar registration with no participant line</v>
+      </c>
+      <c r="J96" s="22" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0408] Post closed seminar registration with no participant line</v>
+      </c>
+      <c r="K96" s="23" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0408 'Post closed seminar registration with no participant line' {</v>
+      </c>
+      <c r="L96" s="20"/>
+    </row>
+    <row r="97" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>16</v>
+      </c>
+      <c r="B97" t="s">
+        <v>26</v>
+      </c>
+      <c r="D97" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F97" t="s">
+        <v>11</v>
+      </c>
+      <c r="G97" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H97" s="12">
+        <v>408</v>
+      </c>
+      <c r="I97" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Seminar</v>
+      </c>
+      <c r="J97" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Seminar</v>
+      </c>
+      <c r="K97" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Seminar'</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>16</v>
+      </c>
+      <c r="B98" t="s">
+        <v>26</v>
+      </c>
+      <c r="D98" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F98" t="s">
+        <v>11</v>
+      </c>
+      <c r="G98" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="H98" s="12">
+        <v>408</v>
+      </c>
+      <c r="I98" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Instructor resource</v>
+      </c>
+      <c r="J98" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Instructor resource</v>
+      </c>
+      <c r="K98" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Instructor resource'</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>16</v>
+      </c>
+      <c r="B99" t="s">
+        <v>26</v>
+      </c>
+      <c r="D99" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F99" t="s">
+        <v>11</v>
+      </c>
+      <c r="G99" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H99" s="12">
+        <v>408</v>
+      </c>
+      <c r="I99" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Room resource</v>
+      </c>
+      <c r="J99" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Room resource</v>
+      </c>
+      <c r="K99" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Room resource'</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>16</v>
+      </c>
+      <c r="B100" t="s">
+        <v>26</v>
+      </c>
+      <c r="D100" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F100" t="s">
+        <v>11</v>
+      </c>
+      <c r="G100" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="H100" s="12">
+        <v>408</v>
+      </c>
+      <c r="I100" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Closed seminar registration with no participant line</v>
+      </c>
+      <c r="J100" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Closed seminar registration with no participant line</v>
+      </c>
+      <c r="K100" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Closed seminar registration with no participant line'</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>16</v>
+      </c>
+      <c r="B101" t="s">
+        <v>26</v>
+      </c>
+      <c r="D101" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F101" t="s">
+        <v>12</v>
+      </c>
+      <c r="G101" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H101" s="12">
+        <v>408</v>
+      </c>
+      <c r="I101" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Post seminar registration</v>
+      </c>
+      <c r="J101" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Post seminar registration</v>
+      </c>
+      <c r="K101" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Post seminar registration'</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>16</v>
+      </c>
+      <c r="B102" t="s">
+        <v>26</v>
+      </c>
+      <c r="D102" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F102" t="s">
+        <v>13</v>
+      </c>
+      <c r="G102" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H102" s="12">
+        <v>408</v>
+      </c>
+      <c r="I102" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[THEN] Error thrown</v>
       </c>
-      <c r="J94" s="13" t="str">
+      <c r="J102" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
         <v>//[THEN] Error thrown</v>
       </c>
-      <c r="K94" s="14" t="str">
+      <c r="K102" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Then 'Error thrown' }</v>
       </c>
     </row>
-    <row r="95" spans="1:12" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="E95" t="s">
+    <row r="103" spans="1:12" ht="45" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B103" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C103" s="19"/>
+      <c r="D103" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E103" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="F103" s="18"/>
+      <c r="G103" s="20"/>
+      <c r="H103" s="21">
+        <v>409</v>
+      </c>
+      <c r="I103" s="20" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0409] Post closed seminar registration with participant line with empty bill-to customer number</v>
+      </c>
+      <c r="J103" s="22" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0409] Post closed seminar registration with participant line with empty bill-to customer number</v>
+      </c>
+      <c r="K103" s="23" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0409 'Post closed seminar registration with participant line with empty bill-to customer number' {</v>
+      </c>
+      <c r="L103" s="20"/>
+    </row>
+    <row r="104" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>16</v>
+      </c>
+      <c r="B104" t="s">
+        <v>26</v>
+      </c>
+      <c r="D104" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F104" t="s">
+        <v>11</v>
+      </c>
+      <c r="G104" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H104" s="12">
+        <v>409</v>
+      </c>
+      <c r="I104" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Seminar</v>
+      </c>
+      <c r="J104" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Seminar</v>
+      </c>
+      <c r="K104" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Seminar'</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>16</v>
+      </c>
+      <c r="B105" t="s">
+        <v>26</v>
+      </c>
+      <c r="D105" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F105" t="s">
+        <v>11</v>
+      </c>
+      <c r="G105" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="H105" s="12">
+        <v>409</v>
+      </c>
+      <c r="I105" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Instructor resource</v>
+      </c>
+      <c r="J105" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Instructor resource</v>
+      </c>
+      <c r="K105" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Instructor resource'</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>16</v>
+      </c>
+      <c r="B106" t="s">
+        <v>26</v>
+      </c>
+      <c r="D106" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F106" t="s">
+        <v>11</v>
+      </c>
+      <c r="G106" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H106" s="12">
+        <v>409</v>
+      </c>
+      <c r="I106" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Room resource</v>
+      </c>
+      <c r="J106" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Room resource</v>
+      </c>
+      <c r="K106" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Room resource'</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>16</v>
+      </c>
+      <c r="B107" t="s">
+        <v>26</v>
+      </c>
+      <c r="D107" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F107" t="s">
+        <v>11</v>
+      </c>
+      <c r="G107" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="H107" s="12">
+        <v>409</v>
+      </c>
+      <c r="I107" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Closed seminar registration with one participant line with empty bill-to customer number</v>
+      </c>
+      <c r="J107" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Closed seminar registration with one participant line with empty bill-to customer number</v>
+      </c>
+      <c r="K107" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Closed seminar registration with one participant line with empty bill-to customer number'</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>16</v>
+      </c>
+      <c r="B108" t="s">
+        <v>26</v>
+      </c>
+      <c r="D108" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F108" t="s">
+        <v>12</v>
+      </c>
+      <c r="G108" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H108" s="12">
+        <v>409</v>
+      </c>
+      <c r="I108" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Post seminar registration</v>
+      </c>
+      <c r="J108" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Post seminar registration</v>
+      </c>
+      <c r="K108" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Post seminar registration'</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>16</v>
+      </c>
+      <c r="B109" t="s">
+        <v>26</v>
+      </c>
+      <c r="D109" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F109" t="s">
+        <v>13</v>
+      </c>
+      <c r="G109" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H109" s="12">
+        <v>409</v>
+      </c>
+      <c r="I109" s="11" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Error thrown</v>
+      </c>
+      <c r="J109" s="13" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Error thrown</v>
+      </c>
+      <c r="K109" s="14" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Error thrown' }</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" ht="45" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B110" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C110" s="19"/>
+      <c r="D110" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E110" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="I95" s="11" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0000] Bill-to Customer empty</v>
-      </c>
-      <c r="J95" s="13" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0000] Bill-to Customer empty</v>
-      </c>
-      <c r="K95" s="14" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0000 'Bill-to Customer empty' {</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E96" t="s">
-        <v>123</v>
-      </c>
-      <c r="I96" s="11" t="str">
-        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
-        <v>[SCENARIO #0000] Participant empty</v>
-      </c>
-      <c r="J96" s="13" t="str">
-        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
-        <v>//[SCENARIO #0000] Participant empty</v>
-      </c>
-      <c r="K96" s="14" t="str">
-        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
-        <v>Scenario 0000 'Participant empty' {</v>
-      </c>
-    </row>
+      <c r="F110" s="18"/>
+      <c r="G110" s="20"/>
+      <c r="H110" s="21">
+        <v>410</v>
+      </c>
+      <c r="I110" s="20" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[SCENARIO #0410] Post closed seminar registration with participant line with empty participant number</v>
+      </c>
+      <c r="J110" s="22" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[SCENARIO #0410] Post closed seminar registration with participant line with empty participant number</v>
+      </c>
+      <c r="K110" s="23" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Scenario 0410 'Post closed seminar registration with participant line with empty participant number' {</v>
+      </c>
+      <c r="L110" s="20"/>
+    </row>
+    <row r="111" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>16</v>
+      </c>
+      <c r="B111" t="s">
+        <v>26</v>
+      </c>
+      <c r="D111" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E111" s="24"/>
+      <c r="F111" t="s">
+        <v>11</v>
+      </c>
+      <c r="G111" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H111" s="12">
+        <v>410</v>
+      </c>
+      <c r="I111" s="25" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Seminar</v>
+      </c>
+      <c r="J111" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Seminar</v>
+      </c>
+      <c r="K111" s="27" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Seminar'</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>16</v>
+      </c>
+      <c r="B112" t="s">
+        <v>26</v>
+      </c>
+      <c r="D112" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E112" s="24"/>
+      <c r="F112" t="s">
+        <v>11</v>
+      </c>
+      <c r="G112" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="H112" s="12">
+        <v>410</v>
+      </c>
+      <c r="I112" s="25" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Instructor resource</v>
+      </c>
+      <c r="J112" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Instructor resource</v>
+      </c>
+      <c r="K112" s="27" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Instructor resource'</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>16</v>
+      </c>
+      <c r="B113" t="s">
+        <v>26</v>
+      </c>
+      <c r="D113" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E113" s="24"/>
+      <c r="F113" t="s">
+        <v>11</v>
+      </c>
+      <c r="G113" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H113" s="12">
+        <v>410</v>
+      </c>
+      <c r="I113" s="25" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Room resource</v>
+      </c>
+      <c r="J113" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Room resource</v>
+      </c>
+      <c r="K113" s="27" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Room resource'</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>16</v>
+      </c>
+      <c r="B114" t="s">
+        <v>26</v>
+      </c>
+      <c r="D114" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E114" s="24"/>
+      <c r="F114" t="s">
+        <v>11</v>
+      </c>
+      <c r="G114" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="H114" s="12">
+        <v>410</v>
+      </c>
+      <c r="I114" s="25" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Customer with company contact</v>
+      </c>
+      <c r="J114" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Customer with company contact</v>
+      </c>
+      <c r="K114" s="27" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Customer with company contact'</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>16</v>
+      </c>
+      <c r="B115" t="s">
+        <v>26</v>
+      </c>
+      <c r="D115" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E115" s="24"/>
+      <c r="F115" t="s">
+        <v>11</v>
+      </c>
+      <c r="G115" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="H115" s="12">
+        <v>410</v>
+      </c>
+      <c r="I115" s="25" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[GIVEN] Closed seminar registration with one participant line with empty participant number</v>
+      </c>
+      <c r="J115" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[GIVEN] Closed seminar registration with one participant line with empty participant number</v>
+      </c>
+      <c r="K115" s="27" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Given 'Closed seminar registration with one participant line with empty participant number'</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>16</v>
+      </c>
+      <c r="B116" t="s">
+        <v>26</v>
+      </c>
+      <c r="D116" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E116" s="24"/>
+      <c r="F116" t="s">
+        <v>12</v>
+      </c>
+      <c r="G116" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H116" s="12">
+        <v>410</v>
+      </c>
+      <c r="I116" s="25" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[WHEN] Post seminar registration</v>
+      </c>
+      <c r="J116" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[WHEN] Post seminar registration</v>
+      </c>
+      <c r="K116" s="27" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>When 'Post seminar registration'</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>16</v>
+      </c>
+      <c r="B117" t="s">
+        <v>26</v>
+      </c>
+      <c r="D117" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E117" s="24"/>
+      <c r="F117" t="s">
+        <v>13</v>
+      </c>
+      <c r="G117" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H117" s="12">
+        <v>410</v>
+      </c>
+      <c r="I117" s="25" t="str">
+        <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
+        <v>[THEN] Error thrown</v>
+      </c>
+      <c r="J117" s="26" t="str">
+        <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
+        <v>//[THEN] Error thrown</v>
+      </c>
+      <c r="K117" s="27" t="str">
+        <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
+        <v>Then 'Error thrown' } }</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" collapsed="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="A1:B1048576">
     <cfRule type="containsBlanks" dxfId="11" priority="5">

</xml_diff>

<commit_message>
FIxed some imperfections and added overview of compiler directives
</commit_message>
<xml_diff>
--- a/test/atdd scenarios/Seminar Registration - ATDD Scenarios.xlsx
+++ b/test/atdd scenarios/Seminar Registration - ATDD Scenarios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvvugt\OneDrive\Presentations\DOK\2024\Nordic\Presentation 1 - Tips &amp; Tricks for efficient and effective test automation data setup\Code Examples\Seminar Management\test\atdd scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f2a63c87061b9b9b/Presentations/DOK/2024/Nordic/Presentation 1 - Tips ^0 Tricks for efficient and effective test automation data setup/Code Examples/Seminar Management/test/atdd scenarios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1643C2B1-EA4C-4D1D-97AA-B1BFC59B4C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="13_ncr:1_{1643C2B1-EA4C-4D1D-97AA-B1BFC59B4C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2170B64-504A-436F-AF67-7F7FA6037E41}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27720" windowHeight="16440" xr2:uid="{37BCB399-09BD-4B93-AAF4-793E3BF59A9F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="125">
   <si>
     <t>Feature</t>
   </si>
@@ -502,7 +502,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -567,16 +567,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -875,9 +865,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -915,7 +905,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1021,7 +1011,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1163,7 +1153,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1173,7 +1163,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7684FF22-50C0-48D3-B42F-054142E19464}">
   <dimension ref="A1:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18:H32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2359,6 +2351,9 @@
       <c r="B38" t="s">
         <v>26</v>
       </c>
+      <c r="D38" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F38" t="s">
         <v>11</v>
       </c>
@@ -2645,6 +2640,9 @@
       <c r="B47" t="s">
         <v>26</v>
       </c>
+      <c r="D47" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F47" t="s">
         <v>11</v>
       </c>
@@ -2931,6 +2929,9 @@
       <c r="B56" t="s">
         <v>26</v>
       </c>
+      <c r="D56" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F56" t="s">
         <v>11</v>
       </c>
@@ -3217,6 +3218,9 @@
       <c r="B65" t="s">
         <v>26</v>
       </c>
+      <c r="D65" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F65" t="s">
         <v>11</v>
       </c>
@@ -3503,6 +3507,9 @@
       <c r="B74" t="s">
         <v>26</v>
       </c>
+      <c r="D74" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F74" t="s">
         <v>11</v>
       </c>
@@ -3789,6 +3796,9 @@
       <c r="B83" t="s">
         <v>26</v>
       </c>
+      <c r="D83" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F83" t="s">
         <v>11</v>
       </c>
@@ -4075,6 +4085,9 @@
       <c r="B92" t="s">
         <v>26</v>
       </c>
+      <c r="D92" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="F92" t="s">
         <v>11</v>
       </c>
@@ -4686,7 +4699,6 @@
       <c r="D111" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E111" s="24"/>
       <c r="F111" t="s">
         <v>11</v>
       </c>
@@ -4696,15 +4708,15 @@
       <c r="H111" s="12">
         <v>410</v>
       </c>
-      <c r="I111" s="25" t="str">
+      <c r="I111" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[GIVEN] Seminar</v>
       </c>
-      <c r="J111" s="26" t="str">
+      <c r="J111" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Seminar</v>
       </c>
-      <c r="K111" s="27" t="str">
+      <c r="K111" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Given 'Seminar'</v>
       </c>
@@ -4719,7 +4731,6 @@
       <c r="D112" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E112" s="24"/>
       <c r="F112" t="s">
         <v>11</v>
       </c>
@@ -4729,15 +4740,15 @@
       <c r="H112" s="12">
         <v>410</v>
       </c>
-      <c r="I112" s="25" t="str">
+      <c r="I112" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[GIVEN] Instructor resource</v>
       </c>
-      <c r="J112" s="26" t="str">
+      <c r="J112" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Instructor resource</v>
       </c>
-      <c r="K112" s="27" t="str">
+      <c r="K112" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Given 'Instructor resource'</v>
       </c>
@@ -4752,7 +4763,6 @@
       <c r="D113" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E113" s="24"/>
       <c r="F113" t="s">
         <v>11</v>
       </c>
@@ -4762,15 +4772,15 @@
       <c r="H113" s="12">
         <v>410</v>
       </c>
-      <c r="I113" s="25" t="str">
+      <c r="I113" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[GIVEN] Room resource</v>
       </c>
-      <c r="J113" s="26" t="str">
+      <c r="J113" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Room resource</v>
       </c>
-      <c r="K113" s="27" t="str">
+      <c r="K113" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Given 'Room resource'</v>
       </c>
@@ -4785,7 +4795,6 @@
       <c r="D114" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E114" s="24"/>
       <c r="F114" t="s">
         <v>11</v>
       </c>
@@ -4795,15 +4804,15 @@
       <c r="H114" s="12">
         <v>410</v>
       </c>
-      <c r="I114" s="25" t="str">
+      <c r="I114" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[GIVEN] Customer with company contact</v>
       </c>
-      <c r="J114" s="26" t="str">
+      <c r="J114" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Customer with company contact</v>
       </c>
-      <c r="K114" s="27" t="str">
+      <c r="K114" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Given 'Customer with company contact'</v>
       </c>
@@ -4818,7 +4827,6 @@
       <c r="D115" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E115" s="24"/>
       <c r="F115" t="s">
         <v>11</v>
       </c>
@@ -4828,15 +4836,15 @@
       <c r="H115" s="12">
         <v>410</v>
       </c>
-      <c r="I115" s="25" t="str">
+      <c r="I115" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[GIVEN] Closed seminar registration with one participant line with empty participant number</v>
       </c>
-      <c r="J115" s="26" t="str">
+      <c r="J115" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
         <v>//[GIVEN] Closed seminar registration with one participant line with empty participant number</v>
       </c>
-      <c r="K115" s="27" t="str">
+      <c r="K115" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Given 'Closed seminar registration with one participant line with empty participant number'</v>
       </c>
@@ -4851,7 +4859,6 @@
       <c r="D116" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E116" s="24"/>
       <c r="F116" t="s">
         <v>12</v>
       </c>
@@ -4861,15 +4868,15 @@
       <c r="H116" s="12">
         <v>410</v>
       </c>
-      <c r="I116" s="25" t="str">
+      <c r="I116" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[WHEN] Post seminar registration</v>
       </c>
-      <c r="J116" s="26" t="str">
+      <c r="J116" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
         <v>//[WHEN] Post seminar registration</v>
       </c>
-      <c r="K116" s="27" t="str">
+      <c r="K116" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>When 'Post seminar registration'</v>
       </c>
@@ -4884,7 +4891,6 @@
       <c r="D117" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E117" s="24"/>
       <c r="F117" t="s">
         <v>13</v>
       </c>
@@ -4894,15 +4900,15 @@
       <c r="H117" s="12">
         <v>410</v>
       </c>
-      <c r="I117" s="25" t="str">
+      <c r="I117" s="11" t="str">
         <f>IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",_xlfn.CONCAT("[FEATURE] ",_xlfn.CONCAT(Table293[[#This Row],[Feature]]," ",Table293[[#This Row],[Sub Feature]])),_xlfn.CONCAT("[SCENARIO #",TEXT(Table293[[#This Row],[Scenario '#]],"0000"),"] ",Table293[[#This Row],[Scenario]])),_xlfn.CONCAT("[",UPPER(Table293[[#This Row],[Given-When-Then (Tag)]]),"] ",Table293[[#This Row],[Given-When-Then (Description)]]))</f>
         <v>[THEN] Error thrown</v>
       </c>
-      <c r="J117" s="26" t="str">
+      <c r="J117" s="13" t="str">
         <f>_xlfn.CONCAT("//",Table293[[#This Row],[ATDD Format]])</f>
         <v>//[THEN] Error thrown</v>
       </c>
-      <c r="K117" s="27" t="str">
+      <c r="K117" s="14" t="str">
         <f ca="1">IF(Table293[[#This Row],[Given-When-Then (Tag)]]="",IF(Table293[[#This Row],[Scenario]]="",IF(Table293[[#This Row],[Feature]]&lt;&gt;"",_xlfn.CONCAT("Feature '",Table293[[#This Row],[Feature]],"' {"),""),_xlfn.CONCAT("Scenario ",TEXT(Table293[[#This Row],[Scenario '#]],"0000")," '",Table293[[#This Row],[Scenario]],"' {")),IF(INDIRECT("F" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"'"),IF(INDIRECT("E" &amp; ROW() + 1)&lt;&gt;"",_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' }"),_xlfn.CONCAT(Table293[[#This Row],[Given-When-Then (Tag)]]," '",Table293[[#This Row],[Given-When-Then (Description)]],"' } }"))))</f>
         <v>Then 'Error thrown' } }</v>
       </c>
@@ -4959,7 +4965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26A05CD-DD6F-435A-8EFB-058B6AB8AAF4}">
   <dimension ref="A1:L74"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>

</xml_diff>